<commit_message>
update to .net 5.0
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -996,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1203,6 +1203,16 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1212,16 +1222,67 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1233,26 +1294,11 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1266,15 +1312,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1282,42 +1319,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -29071,7 +29072,7 @@
   <dimension ref="A1:AA1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -29197,6 +29198,9 @@
       <c r="AA3" s="2"/>
     </row>
     <row r="4" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="78">
+        <v>3</v>
+      </c>
       <c r="B4" s="34" t="s">
         <v>53</v>
       </c>
@@ -29229,8 +29233,8 @@
       <c r="AA4" s="2"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1">
-      <c r="A5" s="30">
-        <v>3</v>
+      <c r="A5" s="78">
+        <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>46</v>
@@ -29268,6 +29272,9 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="78">
+        <v>5</v>
+      </c>
       <c r="B6" s="34" t="s">
         <v>115</v>
       </c>
@@ -29300,6 +29307,9 @@
       <c r="AA6" s="2"/>
     </row>
     <row r="7" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A7" s="78">
+        <v>6</v>
+      </c>
       <c r="B7" s="34" t="s">
         <v>119</v>
       </c>
@@ -29332,8 +29342,8 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
-      <c r="A8" s="30">
-        <v>4</v>
+      <c r="A8" s="78">
+        <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>47</v>
@@ -29371,6 +29381,9 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="78">
+        <v>8</v>
+      </c>
       <c r="B9" s="34" t="s">
         <v>51</v>
       </c>
@@ -29403,8 +29416,8 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1">
-      <c r="A10" s="52">
-        <v>5</v>
+      <c r="A10" s="78">
+        <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>52</v>
@@ -29438,8 +29451,8 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1">
-      <c r="A11" s="52">
-        <v>6</v>
+      <c r="A11" s="78">
+        <v>10</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>156</v>
@@ -29473,6 +29486,9 @@
       <c r="AA11" s="2"/>
     </row>
     <row r="12" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="78">
+        <v>11</v>
+      </c>
       <c r="B12" s="34" t="s">
         <v>158</v>
       </c>
@@ -29505,8 +29521,8 @@
       <c r="AA12" s="2"/>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1">
-      <c r="A13" s="52">
-        <v>7</v>
+      <c r="A13" s="78">
+        <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>55</v>
@@ -29540,6 +29556,9 @@
       <c r="AA13" s="2"/>
     </row>
     <row r="14" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A14" s="78">
+        <v>13</v>
+      </c>
       <c r="B14" s="34" t="s">
         <v>56</v>
       </c>
@@ -29572,6 +29591,9 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A15" s="78">
+        <v>14</v>
+      </c>
       <c r="B15" s="34" t="s">
         <v>63</v>
       </c>
@@ -29604,6 +29626,9 @@
       <c r="AA15" s="2"/>
     </row>
     <row r="16" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="78">
+        <v>15</v>
+      </c>
       <c r="B16" s="34" t="s">
         <v>62</v>
       </c>
@@ -29636,6 +29661,9 @@
       <c r="AA16" s="2"/>
     </row>
     <row r="17" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A17" s="78">
+        <v>16</v>
+      </c>
       <c r="B17" s="34" t="s">
         <v>59</v>
       </c>
@@ -29668,6 +29696,9 @@
       <c r="AA17" s="2"/>
     </row>
     <row r="18" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A18" s="78">
+        <v>17</v>
+      </c>
       <c r="B18" s="34" t="s">
         <v>60</v>
       </c>
@@ -29700,6 +29731,9 @@
       <c r="AA18" s="2"/>
     </row>
     <row r="19" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A19" s="78">
+        <v>18</v>
+      </c>
       <c r="B19" s="34" t="s">
         <v>61</v>
       </c>
@@ -29732,6 +29766,9 @@
       <c r="AA19" s="2"/>
     </row>
     <row r="20" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="78">
+        <v>19</v>
+      </c>
       <c r="B20" s="34" t="s">
         <v>54</v>
       </c>
@@ -29764,6 +29801,9 @@
       <c r="AA20" s="2"/>
     </row>
     <row r="21" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A21" s="78">
+        <v>20</v>
+      </c>
       <c r="B21" s="34" t="s">
         <v>58</v>
       </c>
@@ -29796,6 +29836,9 @@
       <c r="AA21" s="2"/>
     </row>
     <row r="22" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="78">
+        <v>21</v>
+      </c>
       <c r="B22" s="34" t="s">
         <v>57</v>
       </c>
@@ -29828,6 +29871,9 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A23" s="78">
+        <v>22</v>
+      </c>
       <c r="B23" s="34" t="s">
         <v>86</v>
       </c>
@@ -29860,8 +29906,8 @@
       <c r="AA23" s="2"/>
     </row>
     <row r="24" spans="1:27" ht="15" customHeight="1">
-      <c r="A24" s="52">
-        <v>8</v>
+      <c r="A24" s="78">
+        <v>23</v>
       </c>
       <c r="B24" s="34" t="s">
         <v>49</v>
@@ -29895,8 +29941,8 @@
       <c r="AA24" s="2"/>
     </row>
     <row r="25" spans="1:27" ht="15" customHeight="1">
-      <c r="A25" s="52">
-        <v>9</v>
+      <c r="A25" s="78">
+        <v>24</v>
       </c>
       <c r="B25" s="34" t="s">
         <v>50</v>
@@ -29930,8 +29976,8 @@
       <c r="AA25" s="2"/>
     </row>
     <row r="26" spans="1:27" ht="15" customHeight="1">
-      <c r="A26" s="52">
-        <v>10</v>
+      <c r="A26" s="78">
+        <v>25</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>172</v>
@@ -29965,6 +30011,9 @@
       <c r="AA26" s="2"/>
     </row>
     <row r="27" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A27" s="78">
+        <v>26</v>
+      </c>
       <c r="B27" s="34" t="s">
         <v>173</v>
       </c>
@@ -29997,6 +30046,9 @@
       <c r="AA27" s="2"/>
     </row>
     <row r="28" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A28" s="78">
+        <v>27</v>
+      </c>
       <c r="B28" s="34" t="s">
         <v>174</v>
       </c>
@@ -30029,6 +30081,9 @@
       <c r="AA28" s="2"/>
     </row>
     <row r="29" spans="1:27" s="77" customFormat="1" ht="15" customHeight="1">
+      <c r="A29" s="78">
+        <v>28</v>
+      </c>
       <c r="B29" s="34" t="s">
         <v>215</v>
       </c>
@@ -30061,6 +30116,9 @@
       <c r="AA29" s="2"/>
     </row>
     <row r="30" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
+      <c r="A30" s="78">
+        <v>29</v>
+      </c>
       <c r="B30" s="34" t="s">
         <v>175</v>
       </c>
@@ -30093,8 +30151,8 @@
       <c r="AA30" s="2"/>
     </row>
     <row r="31" spans="1:27" ht="15" customHeight="1">
-      <c r="A31" s="52">
-        <v>11</v>
+      <c r="A31" s="78">
+        <v>30</v>
       </c>
       <c r="B31" s="34" t="s">
         <v>70</v>
@@ -30128,6 +30186,9 @@
       <c r="AA31" s="2"/>
     </row>
     <row r="32" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A32" s="78">
+        <v>31</v>
+      </c>
       <c r="B32" s="34" t="s">
         <v>116</v>
       </c>
@@ -30160,6 +30221,9 @@
       <c r="AA32" s="2"/>
     </row>
     <row r="33" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
+      <c r="A33" s="78">
+        <v>32</v>
+      </c>
       <c r="B33" s="34" t="s">
         <v>178</v>
       </c>
@@ -30192,6 +30256,9 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" s="78">
+        <v>33</v>
+      </c>
       <c r="B34" s="34" t="s">
         <v>117</v>
       </c>
@@ -30224,6 +30291,9 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+      <c r="A35" s="78">
+        <v>34</v>
+      </c>
       <c r="B35" s="34" t="s">
         <v>73</v>
       </c>
@@ -30256,8 +30326,8 @@
       <c r="AA35" s="2"/>
     </row>
     <row r="36" spans="1:27" ht="14.4" customHeight="1">
-      <c r="A36" s="52">
-        <v>12</v>
+      <c r="A36" s="78">
+        <v>35</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>72</v>
@@ -30291,8 +30361,8 @@
       <c r="AA36" s="2"/>
     </row>
     <row r="37" spans="1:27" ht="13.2" customHeight="1">
-      <c r="A37" s="52">
-        <v>13</v>
+      <c r="A37" s="78">
+        <v>36</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>71</v>
@@ -30326,6 +30396,9 @@
       <c r="AA37" s="2"/>
     </row>
     <row r="38" spans="1:27" s="65" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A38" s="78">
+        <v>37</v>
+      </c>
       <c r="B38" s="34" t="s">
         <v>85</v>
       </c>
@@ -30358,6 +30431,9 @@
       <c r="AA38" s="2"/>
     </row>
     <row r="39" spans="1:27" s="65" customFormat="1" ht="13.2" customHeight="1">
+      <c r="A39" s="78">
+        <v>38</v>
+      </c>
       <c r="B39" s="34" t="s">
         <v>74</v>
       </c>
@@ -30390,8 +30466,8 @@
       <c r="AA39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="13.8" customHeight="1">
-      <c r="A40" s="52">
-        <v>14</v>
+      <c r="A40" s="78">
+        <v>39</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>75</v>
@@ -30425,8 +30501,8 @@
       <c r="AA40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="15.6" customHeight="1">
-      <c r="A41" s="52">
-        <v>15</v>
+      <c r="A41" s="78">
+        <v>40</v>
       </c>
       <c r="B41" s="34" t="s">
         <v>64</v>
@@ -30460,8 +30536,8 @@
       <c r="AA41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="13.2" customHeight="1">
-      <c r="A42" s="52">
-        <v>16</v>
+      <c r="A42" s="78">
+        <v>41</v>
       </c>
       <c r="B42" s="34" t="s">
         <v>65</v>
@@ -30495,8 +30571,8 @@
       <c r="AA42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="16.8" customHeight="1">
-      <c r="A43" s="52">
-        <v>17</v>
+      <c r="A43" s="78">
+        <v>42</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>66</v>
@@ -30530,8 +30606,8 @@
       <c r="AA43" s="2"/>
     </row>
     <row r="44" spans="1:27" ht="16.2" customHeight="1">
-      <c r="A44" s="52">
-        <v>18</v>
+      <c r="A44" s="78">
+        <v>43</v>
       </c>
       <c r="B44" s="34" t="s">
         <v>69</v>
@@ -30565,6 +30641,9 @@
       <c r="AA44" s="2"/>
     </row>
     <row r="45" spans="1:27" s="65" customFormat="1" ht="16.2" customHeight="1">
+      <c r="A45" s="78">
+        <v>44</v>
+      </c>
       <c r="B45" s="34" t="s">
         <v>113</v>
       </c>
@@ -30597,8 +30676,8 @@
       <c r="AA45" s="2"/>
     </row>
     <row r="46" spans="1:27" ht="13.8" customHeight="1">
-      <c r="A46" s="52">
-        <v>21</v>
+      <c r="A46" s="78">
+        <v>45</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>67</v>
@@ -30632,6 +30711,9 @@
       <c r="AA46" s="2"/>
     </row>
     <row r="47" spans="1:27" ht="13.2" customHeight="1">
+      <c r="A47" s="78">
+        <v>46</v>
+      </c>
       <c r="B47" s="34" t="s">
         <v>68</v>
       </c>
@@ -30664,6 +30746,9 @@
       <c r="AA47" s="2"/>
     </row>
     <row r="48" spans="1:27" ht="13.8" customHeight="1">
+      <c r="A48" s="78">
+        <v>47</v>
+      </c>
       <c r="B48" s="34" t="s">
         <v>76</v>
       </c>
@@ -30695,7 +30780,10 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="2:27" s="77" customFormat="1" ht="13.8" customHeight="1">
+    <row r="49" spans="1:27" s="77" customFormat="1" ht="13.8" customHeight="1">
+      <c r="A49" s="78">
+        <v>48</v>
+      </c>
       <c r="B49" s="34" t="s">
         <v>214</v>
       </c>
@@ -30727,7 +30815,10 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="2:27" ht="15" customHeight="1">
+    <row r="50" spans="1:27" ht="15" customHeight="1">
+      <c r="A50" s="78">
+        <v>49</v>
+      </c>
       <c r="B50" s="34" t="s">
         <v>77</v>
       </c>
@@ -30759,7 +30850,10 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" spans="2:27" ht="13.8" customHeight="1">
+    <row r="51" spans="1:27" ht="13.8" customHeight="1">
+      <c r="A51" s="78">
+        <v>50</v>
+      </c>
       <c r="B51" s="34" t="s">
         <v>114</v>
       </c>
@@ -30791,7 +30885,10 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" spans="2:27" ht="16.2" customHeight="1">
+    <row r="52" spans="1:27" ht="16.2" customHeight="1">
+      <c r="A52" s="78">
+        <v>51</v>
+      </c>
       <c r="B52" s="34" t="s">
         <v>79</v>
       </c>
@@ -30823,7 +30920,10 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" spans="2:27" ht="13.8">
+    <row r="53" spans="1:27" ht="13.8">
+      <c r="A53" s="78">
+        <v>52</v>
+      </c>
       <c r="B53" s="68" t="s">
         <v>80</v>
       </c>
@@ -30855,7 +30955,10 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="2:27" s="65" customFormat="1" ht="13.8">
+    <row r="54" spans="1:27" s="65" customFormat="1" ht="13.8">
+      <c r="A54" s="78">
+        <v>53</v>
+      </c>
       <c r="B54" s="68" t="s">
         <v>88</v>
       </c>
@@ -30887,7 +30990,10 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="2:27" s="65" customFormat="1" ht="13.8">
+    <row r="55" spans="1:27" s="65" customFormat="1" ht="13.8">
+      <c r="A55" s="78">
+        <v>54</v>
+      </c>
       <c r="B55" s="68" t="s">
         <v>83</v>
       </c>
@@ -30919,7 +31025,10 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="2:27" s="65" customFormat="1" ht="13.8">
+    <row r="56" spans="1:27" s="65" customFormat="1" ht="13.8">
+      <c r="A56" s="78">
+        <v>55</v>
+      </c>
       <c r="B56" s="68" t="s">
         <v>94</v>
       </c>
@@ -30951,7 +31060,10 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="2:27" s="66" customFormat="1" ht="13.8">
+    <row r="57" spans="1:27" s="66" customFormat="1" ht="13.8">
+      <c r="A57" s="78">
+        <v>56</v>
+      </c>
       <c r="B57" s="68" t="s">
         <v>212</v>
       </c>
@@ -30983,7 +31095,10 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="2:27" ht="13.8">
+    <row r="58" spans="1:27" ht="13.8">
+      <c r="A58" s="78">
+        <v>57</v>
+      </c>
       <c r="B58" s="2" t="s">
         <v>81</v>
       </c>
@@ -31015,7 +31130,10 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" spans="2:27" s="77" customFormat="1" ht="13.8">
+    <row r="59" spans="1:27" s="77" customFormat="1" ht="13.8">
+      <c r="A59" s="78">
+        <v>58</v>
+      </c>
       <c r="B59" s="68" t="s">
         <v>217</v>
       </c>
@@ -31047,7 +31165,10 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" spans="2:27" s="77" customFormat="1" ht="13.8">
+    <row r="60" spans="1:27" s="77" customFormat="1" ht="13.8">
+      <c r="A60" s="78">
+        <v>59</v>
+      </c>
       <c r="B60" s="68" t="s">
         <v>82</v>
       </c>
@@ -31079,7 +31200,10 @@
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" spans="2:27" ht="13.8">
+    <row r="61" spans="1:27" ht="13.8">
+      <c r="A61" s="78">
+        <v>60</v>
+      </c>
       <c r="B61" s="68" t="s">
         <v>216</v>
       </c>
@@ -31111,7 +31235,10 @@
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" spans="2:27" ht="13.8">
+    <row r="62" spans="1:27" ht="13.8">
+      <c r="A62" s="78">
+        <v>61</v>
+      </c>
       <c r="B62" s="2" t="s">
         <v>84</v>
       </c>
@@ -31143,7 +31270,7 @@
       <c r="Z62" s="2"/>
       <c r="AA62" s="2"/>
     </row>
-    <row r="63" spans="2:27" ht="13.2">
+    <row r="63" spans="1:27" ht="13.2">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -31171,7 +31298,7 @@
       <c r="Z63" s="2"/>
       <c r="AA63" s="2"/>
     </row>
-    <row r="64" spans="2:27" ht="13.2">
+    <row r="64" spans="1:27" ht="13.2">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -58283,13 +58410,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="103" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="115" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="42" t="s">
@@ -58298,14 +58425,14 @@
       <c r="E6" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="81" t="s">
+      <c r="F6" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="49"/>
-      <c r="H6" s="102">
+      <c r="H6" s="115">
         <v>4</v>
       </c>
-      <c r="I6" s="92">
+      <c r="I6" s="87">
         <v>7</v>
       </c>
       <c r="J6" s="39">
@@ -58313,67 +58440,67 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A7" s="84"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="103"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="116"/>
       <c r="D7" s="42" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="82"/>
+      <c r="F7" s="80"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="103"/>
-      <c r="I7" s="93"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="89"/>
       <c r="J7" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A8" s="84"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="103"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="116"/>
       <c r="D8" s="57" t="s">
         <v>102</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="82"/>
+      <c r="F8" s="80"/>
       <c r="G8" s="56"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="93"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="89"/>
       <c r="J8" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="117"/>
       <c r="D9" s="45" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="83"/>
+      <c r="F9" s="81"/>
       <c r="G9" s="50"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="94"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="88"/>
       <c r="J9" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="82" t="s">
         <v>213</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -58382,14 +58509,14 @@
       <c r="E10" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="49"/>
-      <c r="H10" s="99">
+      <c r="H10" s="85">
         <v>4</v>
       </c>
-      <c r="I10" s="92">
+      <c r="I10" s="87">
         <v>8</v>
       </c>
       <c r="J10" s="75">
@@ -58397,85 +58524,85 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A11" s="84"/>
-      <c r="B11" s="82"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="71" t="s">
         <v>107</v>
       </c>
       <c r="E11" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="F11" s="82"/>
+      <c r="F11" s="80"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="93"/>
+      <c r="H11" s="93"/>
+      <c r="I11" s="89"/>
       <c r="J11" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A12" s="84"/>
-      <c r="B12" s="82"/>
-      <c r="C12" s="79"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="71" t="s">
         <v>111</v>
       </c>
       <c r="E12" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="F12" s="82"/>
+      <c r="F12" s="80"/>
       <c r="G12" s="49"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="93"/>
+      <c r="H12" s="93"/>
+      <c r="I12" s="89"/>
       <c r="J12" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A13" s="84"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="79"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="71" t="s">
         <v>105</v>
       </c>
       <c r="E13" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="F13" s="82"/>
+      <c r="F13" s="80"/>
       <c r="G13" s="50"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="93"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="89"/>
       <c r="J13" s="75">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A14" s="89"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="80"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="59" t="s">
         <v>149</v>
       </c>
       <c r="E14" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="F14" s="83"/>
+      <c r="F14" s="81"/>
       <c r="G14" s="70"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="94"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="88"/>
       <c r="J14" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="82" t="s">
         <v>98</v>
       </c>
       <c r="D15" s="35" t="s">
@@ -58484,14 +58611,14 @@
       <c r="E15" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="49"/>
-      <c r="H15" s="99">
+      <c r="H15" s="85">
         <v>3</v>
       </c>
-      <c r="I15" s="92">
+      <c r="I15" s="87">
         <v>6</v>
       </c>
       <c r="J15" s="66">
@@ -58499,67 +58626,67 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A16" s="97"/>
-      <c r="B16" s="82"/>
-      <c r="C16" s="79"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="62" t="s">
         <v>122</v>
       </c>
       <c r="E16" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="82"/>
+      <c r="F16" s="80"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="93"/>
+      <c r="H16" s="93"/>
+      <c r="I16" s="89"/>
       <c r="J16" s="66">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A17" s="97"/>
-      <c r="B17" s="82"/>
-      <c r="C17" s="79"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="80"/>
+      <c r="C17" s="83"/>
       <c r="D17" s="62" t="s">
         <v>129</v>
       </c>
       <c r="E17" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="82"/>
+      <c r="F17" s="80"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="89"/>
       <c r="J17" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A18" s="98"/>
-      <c r="B18" s="83"/>
-      <c r="C18" s="80"/>
+      <c r="A18" s="114"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="84"/>
       <c r="D18" s="48" t="s">
         <v>123</v>
       </c>
       <c r="E18" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="F18" s="83"/>
+      <c r="F18" s="81"/>
       <c r="G18" s="50"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="94"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="88"/>
       <c r="J18" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="104" t="s">
         <v>132</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="82" t="s">
         <v>120</v>
       </c>
       <c r="D19" s="54" t="s">
@@ -58568,14 +58695,14 @@
       <c r="E19" s="72" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="81" t="s">
+      <c r="F19" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G19" s="70"/>
-      <c r="H19" s="99">
+      <c r="H19" s="85">
         <v>2</v>
       </c>
-      <c r="I19" s="92">
+      <c r="I19" s="87">
         <v>3</v>
       </c>
       <c r="J19" s="66">
@@ -58583,31 +58710,31 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A20" s="84"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="79"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="83"/>
       <c r="D20" s="54" t="s">
         <v>130</v>
       </c>
       <c r="E20" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="83"/>
+      <c r="F20" s="81"/>
       <c r="G20" s="70"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="94"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="88"/>
       <c r="J20" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A21" s="88" t="s">
+      <c r="A21" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="82" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="36" t="s">
@@ -58616,14 +58743,14 @@
       <c r="E21" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="F21" s="81" t="s">
+      <c r="F21" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="49"/>
-      <c r="H21" s="99">
+      <c r="H21" s="85">
         <v>3</v>
       </c>
-      <c r="I21" s="92">
+      <c r="I21" s="87">
         <v>5</v>
       </c>
       <c r="J21" s="66">
@@ -58631,63 +58758,63 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="79"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="83"/>
       <c r="D22" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="90" t="s">
+      <c r="E22" s="101" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="82"/>
+      <c r="F22" s="80"/>
       <c r="G22" s="49"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="89"/>
       <c r="J22" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A23" s="84"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="80"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="84"/>
       <c r="D23" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="E23" s="95"/>
-      <c r="F23" s="83"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="81"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="94"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="88"/>
       <c r="J23" s="66">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="103" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="78" t="s">
+      <c r="C24" s="82" t="s">
         <v>139</v>
       </c>
       <c r="D24" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="E24" s="85" t="s">
+      <c r="E24" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="F24" s="81" t="s">
+      <c r="F24" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="49"/>
-      <c r="H24" s="99">
+      <c r="H24" s="85">
         <v>3</v>
       </c>
-      <c r="I24" s="92">
+      <c r="I24" s="87">
         <v>5</v>
       </c>
       <c r="J24" s="76">
@@ -58712,17 +58839,17 @@
       <c r="AA24" s="18"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="84"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="79"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="E25" s="86"/>
-      <c r="F25" s="82"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="80"/>
       <c r="G25" s="50"/>
-      <c r="H25" s="100"/>
-      <c r="I25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="89"/>
       <c r="J25" s="76">
         <v>2</v>
       </c>
@@ -58745,17 +58872,17 @@
       <c r="AA25" s="18"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A26" s="89"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="80"/>
+      <c r="A26" s="105"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="84"/>
       <c r="D26" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="83"/>
+      <c r="E26" s="108"/>
+      <c r="F26" s="81"/>
       <c r="G26" s="51"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="94"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="88"/>
       <c r="J26" s="76">
         <v>2</v>
       </c>
@@ -58778,27 +58905,27 @@
       <c r="AA26" s="18"/>
     </row>
     <row r="27" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="103" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="81" t="s">
+      <c r="B27" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="82" t="s">
         <v>144</v>
       </c>
       <c r="D27" s="54" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="85" t="s">
+      <c r="E27" s="106" t="s">
         <v>153</v>
       </c>
       <c r="F27" s="63"/>
       <c r="G27" s="70"/>
-      <c r="H27" s="110">
+      <c r="H27" s="90">
         <v>2</v>
       </c>
-      <c r="I27" s="92">
+      <c r="I27" s="87">
         <v>4</v>
       </c>
       <c r="J27" s="76">
@@ -58823,19 +58950,19 @@
       <c r="AA27" s="18"/>
     </row>
     <row r="28" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A28" s="84"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="79"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="80"/>
+      <c r="C28" s="83"/>
       <c r="D28" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="E28" s="86"/>
+      <c r="E28" s="107"/>
       <c r="F28" s="63" t="s">
         <v>39</v>
       </c>
       <c r="G28" s="70"/>
-      <c r="H28" s="111"/>
-      <c r="I28" s="93"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="89"/>
       <c r="J28" s="76">
         <v>1</v>
       </c>
@@ -58858,17 +58985,17 @@
       <c r="AA28" s="18"/>
     </row>
     <row r="29" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="89"/>
-      <c r="B29" s="83"/>
-      <c r="C29" s="80"/>
+      <c r="A29" s="105"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="84"/>
       <c r="D29" s="54" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="87"/>
+      <c r="E29" s="108"/>
       <c r="F29" s="63"/>
       <c r="G29" s="70"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="94"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="88"/>
       <c r="J29" s="76">
         <v>2</v>
       </c>
@@ -58891,29 +59018,29 @@
       <c r="AA29" s="18"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A30" s="88" t="s">
+      <c r="A30" s="103" t="s">
         <v>156</v>
       </c>
-      <c r="B30" s="81" t="s">
+      <c r="B30" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="78" t="s">
+      <c r="C30" s="82" t="s">
         <v>93</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="90" t="s">
+      <c r="E30" s="101" t="s">
         <v>155</v>
       </c>
-      <c r="F30" s="81" t="s">
+      <c r="F30" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G30" s="49"/>
-      <c r="H30" s="99">
+      <c r="H30" s="85">
         <v>2</v>
       </c>
-      <c r="I30" s="92">
+      <c r="I30" s="87">
         <v>3</v>
       </c>
       <c r="J30" s="76">
@@ -58938,17 +59065,17 @@
       <c r="AA30" s="18"/>
     </row>
     <row r="31" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="84"/>
-      <c r="B31" s="82"/>
-      <c r="C31" s="79"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="83"/>
       <c r="D31" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="91"/>
-      <c r="F31" s="82"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="80"/>
       <c r="G31" s="49"/>
-      <c r="H31" s="100"/>
-      <c r="I31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="89"/>
       <c r="J31" s="76">
         <v>1</v>
       </c>
@@ -58971,17 +59098,17 @@
       <c r="AA31" s="18"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="84"/>
-      <c r="B32" s="82"/>
-      <c r="C32" s="79"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="83"/>
       <c r="D32" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="E32" s="91"/>
-      <c r="F32" s="83"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="81"/>
       <c r="G32" s="64"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="93"/>
+      <c r="H32" s="93"/>
+      <c r="I32" s="89"/>
       <c r="J32" s="76">
         <v>1</v>
       </c>
@@ -59004,29 +59131,29 @@
       <c r="AA32" s="18"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A33" s="88" t="s">
+      <c r="A33" s="103" t="s">
         <v>158</v>
       </c>
-      <c r="B33" s="81" t="s">
+      <c r="B33" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C33" s="82" t="s">
         <v>92</v>
       </c>
       <c r="D33" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="85" t="s">
+      <c r="E33" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="F33" s="81" t="s">
+      <c r="F33" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="49"/>
-      <c r="H33" s="99">
+      <c r="H33" s="85">
         <v>2</v>
       </c>
-      <c r="I33" s="92">
+      <c r="I33" s="87">
         <v>3</v>
       </c>
       <c r="J33" s="76">
@@ -59051,17 +59178,17 @@
       <c r="AA33" s="18"/>
     </row>
     <row r="34" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="84"/>
-      <c r="B34" s="82"/>
-      <c r="C34" s="79"/>
+      <c r="A34" s="104"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="83"/>
       <c r="D34" s="74" t="s">
         <v>157</v>
       </c>
-      <c r="E34" s="86"/>
-      <c r="F34" s="82"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="80"/>
       <c r="G34" s="49"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="89"/>
       <c r="J34" s="76">
         <v>1</v>
       </c>
@@ -59084,17 +59211,17 @@
       <c r="AA34" s="18"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A35" s="84"/>
-      <c r="B35" s="82"/>
-      <c r="C35" s="79"/>
+      <c r="A35" s="104"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="83"/>
       <c r="D35" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="86"/>
-      <c r="F35" s="82"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="80"/>
       <c r="G35" s="64"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="89"/>
       <c r="J35" s="76">
         <v>1</v>
       </c>
@@ -59117,29 +59244,29 @@
       <c r="AA35" s="18"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="103" t="s">
         <v>90</v>
       </c>
-      <c r="B36" s="81" t="s">
+      <c r="B36" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="78" t="s">
+      <c r="C36" s="82" t="s">
         <v>48</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E36" s="85" t="s">
+      <c r="E36" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="F36" s="81" t="s">
+      <c r="F36" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="49"/>
-      <c r="H36" s="113">
+      <c r="H36" s="97">
         <v>4</v>
       </c>
-      <c r="I36" s="92">
+      <c r="I36" s="87">
         <v>8</v>
       </c>
       <c r="J36" s="76">
@@ -59164,17 +59291,17 @@
       <c r="AA36" s="18"/>
     </row>
     <row r="37" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="84"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="79"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="83"/>
       <c r="D37" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="86"/>
-      <c r="F37" s="82"/>
+      <c r="E37" s="107"/>
+      <c r="F37" s="80"/>
       <c r="G37" s="49"/>
-      <c r="H37" s="114"/>
-      <c r="I37" s="93"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="89"/>
       <c r="J37" s="76">
         <v>1</v>
       </c>
@@ -59197,17 +59324,17 @@
       <c r="AA37" s="18"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="84"/>
-      <c r="B38" s="82"/>
-      <c r="C38" s="79"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="80"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="62" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="86"/>
-      <c r="F38" s="82"/>
+      <c r="E38" s="107"/>
+      <c r="F38" s="80"/>
       <c r="G38" s="50"/>
-      <c r="H38" s="115"/>
-      <c r="I38" s="93"/>
+      <c r="H38" s="99"/>
+      <c r="I38" s="89"/>
       <c r="J38" s="76">
         <v>1</v>
       </c>
@@ -59230,17 +59357,17 @@
       <c r="AA38" s="18"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="89"/>
-      <c r="B39" s="83"/>
-      <c r="C39" s="80"/>
+      <c r="A39" s="105"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="84"/>
       <c r="D39" s="61" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="87"/>
-      <c r="F39" s="83"/>
+      <c r="E39" s="108"/>
+      <c r="F39" s="81"/>
       <c r="G39" s="51"/>
-      <c r="H39" s="116"/>
-      <c r="I39" s="94"/>
+      <c r="H39" s="100"/>
+      <c r="I39" s="88"/>
       <c r="J39" s="76">
         <v>5</v>
       </c>
@@ -59263,29 +59390,29 @@
       <c r="AA39" s="18"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="88" t="s">
+      <c r="A40" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="81" t="s">
+      <c r="B40" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="78" t="s">
+      <c r="C40" s="82" t="s">
         <v>96</v>
       </c>
       <c r="D40" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E40" s="108" t="s">
+      <c r="E40" s="109" t="s">
         <v>96</v>
       </c>
-      <c r="F40" s="81" t="s">
+      <c r="F40" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G40" s="49"/>
-      <c r="H40" s="99">
+      <c r="H40" s="85">
         <v>2</v>
       </c>
-      <c r="I40" s="92">
+      <c r="I40" s="87">
         <v>3</v>
       </c>
       <c r="J40" s="76">
@@ -59310,17 +59437,17 @@
       <c r="AA40" s="18"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="84"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="79"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="80"/>
+      <c r="C41" s="83"/>
       <c r="D41" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="E41" s="109"/>
-      <c r="F41" s="82"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="80"/>
       <c r="G41" s="64"/>
-      <c r="H41" s="100"/>
-      <c r="I41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="89"/>
       <c r="J41" s="76">
         <v>1</v>
       </c>
@@ -59343,29 +59470,29 @@
       <c r="AA41" s="18"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A42" s="88" t="s">
+      <c r="A42" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="81" t="s">
+      <c r="B42" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="78" t="s">
+      <c r="C42" s="82" t="s">
         <v>97</v>
       </c>
       <c r="D42" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="E42" s="90" t="s">
+      <c r="E42" s="101" t="s">
         <v>169</v>
       </c>
-      <c r="F42" s="81" t="s">
+      <c r="F42" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="49"/>
-      <c r="H42" s="99">
+      <c r="H42" s="85">
         <v>2</v>
       </c>
-      <c r="I42" s="92">
+      <c r="I42" s="87">
         <v>3</v>
       </c>
       <c r="J42" s="76">
@@ -59390,17 +59517,17 @@
       <c r="AA42" s="18"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A43" s="84"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="79"/>
+      <c r="A43" s="104"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="83"/>
       <c r="D43" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="E43" s="91"/>
-      <c r="F43" s="83"/>
+      <c r="E43" s="102"/>
+      <c r="F43" s="81"/>
       <c r="G43" s="64"/>
-      <c r="H43" s="100"/>
-      <c r="I43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="89"/>
       <c r="J43" s="76">
         <v>1</v>
       </c>
@@ -59423,29 +59550,29 @@
       <c r="AA43" s="18"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A44" s="88" t="s">
+      <c r="A44" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="B44" s="81" t="s">
+      <c r="B44" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="78" t="s">
+      <c r="C44" s="82" t="s">
         <v>176</v>
       </c>
       <c r="D44" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="E44" s="90" t="s">
+      <c r="E44" s="101" t="s">
         <v>193</v>
       </c>
-      <c r="F44" s="81" t="s">
+      <c r="F44" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="50"/>
-      <c r="H44" s="99">
+      <c r="H44" s="85">
         <v>2</v>
       </c>
-      <c r="I44" s="92">
+      <c r="I44" s="87">
         <v>4</v>
       </c>
       <c r="J44" s="76">
@@ -59470,17 +59597,17 @@
       <c r="AA44" s="18"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="84"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="79"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="E45" s="91"/>
-      <c r="F45" s="82"/>
+      <c r="E45" s="102"/>
+      <c r="F45" s="80"/>
       <c r="G45" s="56"/>
-      <c r="H45" s="100"/>
-      <c r="I45" s="93"/>
+      <c r="H45" s="93"/>
+      <c r="I45" s="89"/>
       <c r="J45" s="76">
         <v>2</v>
       </c>
@@ -59503,29 +59630,29 @@
       <c r="AA45" s="18"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="88" t="s">
+      <c r="A46" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="B46" s="81" t="s">
+      <c r="B46" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="78" t="s">
+      <c r="C46" s="82" t="s">
         <v>177</v>
       </c>
       <c r="D46" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="E46" s="105" t="s">
+      <c r="E46" s="94" t="s">
         <v>192</v>
       </c>
-      <c r="F46" s="81" t="s">
+      <c r="F46" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G46" s="49"/>
-      <c r="H46" s="99">
+      <c r="H46" s="85">
         <v>3</v>
       </c>
-      <c r="I46" s="92">
+      <c r="I46" s="87">
         <v>5</v>
       </c>
       <c r="J46" s="76">
@@ -59550,17 +59677,17 @@
       <c r="AA46" s="18"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="84"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="79"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="83"/>
       <c r="D47" s="62" t="s">
         <v>191</v>
       </c>
-      <c r="E47" s="106"/>
-      <c r="F47" s="82"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="80"/>
       <c r="G47" s="50"/>
-      <c r="H47" s="100"/>
-      <c r="I47" s="93"/>
+      <c r="H47" s="93"/>
+      <c r="I47" s="89"/>
       <c r="J47" s="76">
         <v>2</v>
       </c>
@@ -59583,17 +59710,17 @@
       <c r="AA47" s="18"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A48" s="89"/>
-      <c r="B48" s="83"/>
-      <c r="C48" s="80"/>
+      <c r="A48" s="105"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="84"/>
       <c r="D48" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="E48" s="107"/>
-      <c r="F48" s="83"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="81"/>
       <c r="G48" s="51"/>
-      <c r="H48" s="101"/>
-      <c r="I48" s="94"/>
+      <c r="H48" s="86"/>
+      <c r="I48" s="88"/>
       <c r="J48" s="76">
         <v>1</v>
       </c>
@@ -59616,29 +59743,29 @@
       <c r="AA48" s="18"/>
     </row>
     <row r="49" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A49" s="88" t="s">
+      <c r="A49" s="103" t="s">
         <v>178</v>
       </c>
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="78" t="s">
+      <c r="C49" s="82" t="s">
         <v>179</v>
       </c>
       <c r="D49" s="54" t="s">
         <v>180</v>
       </c>
-      <c r="E49" s="105" t="s">
+      <c r="E49" s="94" t="s">
         <v>183</v>
       </c>
-      <c r="F49" s="81" t="s">
+      <c r="F49" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="99">
+      <c r="H49" s="85">
         <v>3</v>
       </c>
-      <c r="I49" s="92">
+      <c r="I49" s="87">
         <v>6</v>
       </c>
       <c r="J49" s="76">
@@ -59663,17 +59790,17 @@
       <c r="AA49" s="18"/>
     </row>
     <row r="50" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="84"/>
-      <c r="B50" s="82"/>
-      <c r="C50" s="79"/>
+      <c r="A50" s="104"/>
+      <c r="B50" s="80"/>
+      <c r="C50" s="83"/>
       <c r="D50" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="E50" s="106"/>
-      <c r="F50" s="82"/>
+      <c r="E50" s="95"/>
+      <c r="F50" s="80"/>
       <c r="G50" s="70"/>
-      <c r="H50" s="100"/>
-      <c r="I50" s="93"/>
+      <c r="H50" s="93"/>
+      <c r="I50" s="89"/>
       <c r="J50" s="76">
         <v>1</v>
       </c>
@@ -59696,17 +59823,17 @@
       <c r="AA50" s="18"/>
     </row>
     <row r="51" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A51" s="89"/>
-      <c r="B51" s="83"/>
-      <c r="C51" s="80"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="84"/>
       <c r="D51" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="E51" s="107"/>
-      <c r="F51" s="83"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="81"/>
       <c r="G51" s="70"/>
-      <c r="H51" s="101"/>
-      <c r="I51" s="94"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="88"/>
       <c r="J51" s="76">
         <v>4</v>
       </c>
@@ -59729,29 +59856,29 @@
       <c r="AA51" s="18"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A52" s="88" t="s">
+      <c r="A52" s="103" t="s">
         <v>69</v>
       </c>
-      <c r="B52" s="81" t="s">
+      <c r="B52" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="78" t="s">
+      <c r="C52" s="82" t="s">
         <v>194</v>
       </c>
       <c r="D52" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="105" t="s">
+      <c r="E52" s="94" t="s">
         <v>187</v>
       </c>
-      <c r="F52" s="81" t="s">
+      <c r="F52" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G52" s="49"/>
-      <c r="H52" s="99">
+      <c r="H52" s="85">
         <v>2</v>
       </c>
-      <c r="I52" s="92">
+      <c r="I52" s="87">
         <v>4</v>
       </c>
       <c r="J52" s="76">
@@ -59776,17 +59903,17 @@
       <c r="AA52" s="18"/>
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A53" s="84"/>
-      <c r="B53" s="82"/>
-      <c r="C53" s="79"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="80"/>
+      <c r="C53" s="83"/>
       <c r="D53" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="E53" s="106"/>
-      <c r="F53" s="82"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="80"/>
       <c r="G53" s="50"/>
-      <c r="H53" s="100"/>
-      <c r="I53" s="93"/>
+      <c r="H53" s="93"/>
+      <c r="I53" s="89"/>
       <c r="J53" s="76">
         <v>1</v>
       </c>
@@ -59809,17 +59936,17 @@
       <c r="AA53" s="18"/>
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A54" s="89"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="80"/>
+      <c r="A54" s="105"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="84"/>
       <c r="D54" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="E54" s="107"/>
-      <c r="F54" s="83"/>
+      <c r="E54" s="96"/>
+      <c r="F54" s="81"/>
       <c r="G54" s="51"/>
-      <c r="H54" s="101"/>
-      <c r="I54" s="94"/>
+      <c r="H54" s="86"/>
+      <c r="I54" s="88"/>
       <c r="J54" s="76">
         <v>2</v>
       </c>
@@ -59842,27 +59969,27 @@
       <c r="AA54" s="18"/>
     </row>
     <row r="55" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A55" s="88" t="s">
+      <c r="A55" s="103" t="s">
         <v>118</v>
       </c>
       <c r="B55" s="63"/>
-      <c r="C55" s="78" t="s">
+      <c r="C55" s="82" t="s">
         <v>195</v>
       </c>
       <c r="D55" s="54" t="s">
         <v>196</v>
       </c>
-      <c r="E55" s="105" t="s">
+      <c r="E55" s="94" t="s">
         <v>198</v>
       </c>
-      <c r="F55" s="81" t="s">
+      <c r="F55" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G55" s="70"/>
-      <c r="H55" s="99">
+      <c r="H55" s="85">
         <v>2</v>
       </c>
-      <c r="I55" s="92">
+      <c r="I55" s="87">
         <v>3</v>
       </c>
       <c r="J55" s="76">
@@ -59887,19 +60014,19 @@
       <c r="AA55" s="18"/>
     </row>
     <row r="56" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A56" s="84"/>
+      <c r="A56" s="104"/>
       <c r="B56" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="79"/>
+      <c r="C56" s="83"/>
       <c r="D56" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="E56" s="106"/>
-      <c r="F56" s="82"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="80"/>
       <c r="G56" s="70"/>
-      <c r="H56" s="100"/>
-      <c r="I56" s="93"/>
+      <c r="H56" s="93"/>
+      <c r="I56" s="89"/>
       <c r="J56" s="76">
         <v>1</v>
       </c>
@@ -59922,17 +60049,17 @@
       <c r="AA56" s="18"/>
     </row>
     <row r="57" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A57" s="89"/>
+      <c r="A57" s="105"/>
       <c r="B57" s="63"/>
-      <c r="C57" s="80"/>
+      <c r="C57" s="84"/>
       <c r="D57" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="E57" s="107"/>
-      <c r="F57" s="83"/>
+      <c r="E57" s="96"/>
+      <c r="F57" s="81"/>
       <c r="G57" s="70"/>
-      <c r="H57" s="101"/>
-      <c r="I57" s="94"/>
+      <c r="H57" s="86"/>
+      <c r="I57" s="88"/>
       <c r="J57" s="76">
         <v>1</v>
       </c>
@@ -59955,29 +60082,29 @@
       <c r="AA57" s="18"/>
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A58" s="88" t="s">
+      <c r="A58" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="81" t="s">
+      <c r="B58" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="78" t="s">
+      <c r="C58" s="82" t="s">
         <v>99</v>
       </c>
       <c r="D58" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="E58" s="105" t="s">
+      <c r="E58" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="F58" s="81" t="s">
+      <c r="F58" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G58" s="50"/>
-      <c r="H58" s="99">
+      <c r="H58" s="85">
         <v>2</v>
       </c>
-      <c r="I58" s="92">
+      <c r="I58" s="87">
         <v>4</v>
       </c>
       <c r="J58" s="76">
@@ -60002,17 +60129,17 @@
       <c r="AA58" s="18"/>
     </row>
     <row r="59" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="84"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="79"/>
+      <c r="A59" s="104"/>
+      <c r="B59" s="80"/>
+      <c r="C59" s="83"/>
       <c r="D59" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="E59" s="106"/>
-      <c r="F59" s="82"/>
+      <c r="E59" s="95"/>
+      <c r="F59" s="80"/>
       <c r="G59" s="50"/>
-      <c r="H59" s="100"/>
-      <c r="I59" s="93"/>
+      <c r="H59" s="93"/>
+      <c r="I59" s="89"/>
       <c r="J59" s="76">
         <v>2</v>
       </c>
@@ -60035,17 +60162,17 @@
       <c r="AA59" s="18"/>
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A60" s="89"/>
-      <c r="B60" s="83"/>
-      <c r="C60" s="80"/>
+      <c r="A60" s="105"/>
+      <c r="B60" s="81"/>
+      <c r="C60" s="84"/>
       <c r="D60" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="E60" s="107"/>
-      <c r="F60" s="83"/>
+      <c r="E60" s="96"/>
+      <c r="F60" s="81"/>
       <c r="G60" s="70"/>
-      <c r="H60" s="101"/>
-      <c r="I60" s="94"/>
+      <c r="H60" s="86"/>
+      <c r="I60" s="88"/>
       <c r="J60" s="76">
         <v>1</v>
       </c>
@@ -60068,29 +60195,29 @@
       <c r="AA60" s="18"/>
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A61" s="88" t="s">
+      <c r="A61" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="81" t="s">
+      <c r="B61" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="78" t="s">
+      <c r="C61" s="82" t="s">
         <v>100</v>
       </c>
       <c r="D61" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="E61" s="105" t="s">
+      <c r="E61" s="94" t="s">
         <v>207</v>
       </c>
-      <c r="F61" s="81" t="s">
+      <c r="F61" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G61" s="49"/>
-      <c r="H61" s="99">
+      <c r="H61" s="85">
         <v>2</v>
       </c>
-      <c r="I61" s="92">
+      <c r="I61" s="87">
         <v>4</v>
       </c>
       <c r="J61" s="76">
@@ -60115,17 +60242,17 @@
       <c r="AA61" s="18"/>
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A62" s="84"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="79"/>
+      <c r="A62" s="104"/>
+      <c r="B62" s="80"/>
+      <c r="C62" s="83"/>
       <c r="D62" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="E62" s="106"/>
-      <c r="F62" s="82"/>
+      <c r="E62" s="95"/>
+      <c r="F62" s="80"/>
       <c r="G62" s="50"/>
-      <c r="H62" s="100"/>
-      <c r="I62" s="93"/>
+      <c r="H62" s="93"/>
+      <c r="I62" s="89"/>
       <c r="J62" s="76">
         <v>1</v>
       </c>
@@ -60148,17 +60275,17 @@
       <c r="AA62" s="18"/>
     </row>
     <row r="63" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="84"/>
-      <c r="B63" s="82"/>
-      <c r="C63" s="79"/>
+      <c r="A63" s="104"/>
+      <c r="B63" s="80"/>
+      <c r="C63" s="83"/>
       <c r="D63" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="E63" s="106"/>
-      <c r="F63" s="82"/>
+      <c r="E63" s="95"/>
+      <c r="F63" s="80"/>
       <c r="G63" s="50"/>
-      <c r="H63" s="100"/>
-      <c r="I63" s="93"/>
+      <c r="H63" s="93"/>
+      <c r="I63" s="89"/>
       <c r="J63" s="76">
         <v>1</v>
       </c>
@@ -60181,17 +60308,17 @@
       <c r="AA63" s="18"/>
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A64" s="89"/>
-      <c r="B64" s="83"/>
-      <c r="C64" s="80"/>
+      <c r="A64" s="105"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="84"/>
       <c r="D64" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="E64" s="107"/>
-      <c r="F64" s="83"/>
+      <c r="E64" s="96"/>
+      <c r="F64" s="81"/>
       <c r="G64" s="50"/>
-      <c r="H64" s="101"/>
-      <c r="I64" s="94"/>
+      <c r="H64" s="86"/>
+      <c r="I64" s="88"/>
       <c r="J64" s="76">
         <v>1</v>
       </c>
@@ -60214,29 +60341,29 @@
       <c r="AA64" s="18"/>
     </row>
     <row r="65" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A65" s="88" t="s">
+      <c r="A65" s="103" t="s">
         <v>88</v>
       </c>
-      <c r="B65" s="81" t="s">
+      <c r="B65" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="78" t="s">
+      <c r="C65" s="82" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="54" t="s">
         <v>208</v>
       </c>
-      <c r="E65" s="105" t="s">
+      <c r="E65" s="94" t="s">
         <v>211</v>
       </c>
-      <c r="F65" s="81" t="s">
+      <c r="F65" s="79" t="s">
         <v>39</v>
       </c>
       <c r="G65" s="70"/>
-      <c r="H65" s="99">
+      <c r="H65" s="85">
         <v>2</v>
       </c>
-      <c r="I65" s="92">
+      <c r="I65" s="87">
         <v>3</v>
       </c>
       <c r="J65" s="76">
@@ -60261,17 +60388,17 @@
       <c r="AA65" s="18"/>
     </row>
     <row r="66" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A66" s="84"/>
-      <c r="B66" s="82"/>
-      <c r="C66" s="79"/>
+      <c r="A66" s="104"/>
+      <c r="B66" s="80"/>
+      <c r="C66" s="83"/>
       <c r="D66" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="E66" s="106"/>
-      <c r="F66" s="82"/>
+      <c r="E66" s="95"/>
+      <c r="F66" s="80"/>
       <c r="G66" s="50"/>
-      <c r="H66" s="100"/>
-      <c r="I66" s="93"/>
+      <c r="H66" s="93"/>
+      <c r="I66" s="89"/>
       <c r="J66" s="76">
         <v>1</v>
       </c>
@@ -60294,17 +60421,17 @@
       <c r="AA66" s="18"/>
     </row>
     <row r="67" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A67" s="89"/>
-      <c r="B67" s="83"/>
-      <c r="C67" s="80"/>
+      <c r="A67" s="105"/>
+      <c r="B67" s="81"/>
+      <c r="C67" s="84"/>
       <c r="D67" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="E67" s="107"/>
-      <c r="F67" s="83"/>
+      <c r="E67" s="96"/>
+      <c r="F67" s="81"/>
       <c r="G67" s="50"/>
-      <c r="H67" s="101"/>
-      <c r="I67" s="94"/>
+      <c r="H67" s="86"/>
+      <c r="I67" s="88"/>
       <c r="J67" s="76">
         <v>1</v>
       </c>
@@ -64683,6 +64810,116 @@
     <row r="944" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="134">
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="H6:H9"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="H46:H48"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I65:I67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="I58:I60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="H58:H60"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="F58:F60"/>
     <mergeCell ref="F61:F64"/>
     <mergeCell ref="F65:F67"/>
@@ -64707,116 +64944,6 @@
     <mergeCell ref="I42:I43"/>
     <mergeCell ref="I44:I45"/>
     <mergeCell ref="I46:I48"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="I65:I67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="I58:I60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="H58:H60"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="H52:H54"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="H46:H48"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="H6:H9"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A10:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -64845,112 +64972,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="123" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="121"/>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A2" s="121"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
+      <c r="A2" s="122"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A3" s="121"/>
-      <c r="B3" s="121"/>
-      <c r="C3" s="121"/>
-      <c r="D3" s="121"/>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
+      <c r="A3" s="122"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="122"/>
+      <c r="N3" s="122"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A4" s="121"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121"/>
-      <c r="I4" s="121"/>
-      <c r="J4" s="121"/>
-      <c r="K4" s="121"/>
-      <c r="L4" s="121"/>
-      <c r="M4" s="121"/>
-      <c r="N4" s="121"/>
+      <c r="A4" s="122"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
+      <c r="G4" s="122"/>
+      <c r="H4" s="122"/>
+      <c r="I4" s="122"/>
+      <c r="J4" s="122"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
+      <c r="M4" s="122"/>
+      <c r="N4" s="122"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="121"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="121"/>
-      <c r="G5" s="121"/>
-      <c r="H5" s="121"/>
-      <c r="I5" s="121"/>
-      <c r="J5" s="121"/>
-      <c r="K5" s="121"/>
-      <c r="L5" s="121"/>
-      <c r="M5" s="121"/>
-      <c r="N5" s="121"/>
+      <c r="A5" s="122"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="122"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="122"/>
     </row>
     <row r="6" spans="1:14" ht="95.25" customHeight="1">
-      <c r="A6" s="121"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="121"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="119"/>
-      <c r="I7" s="120"/>
-      <c r="J7" s="121"/>
-      <c r="K7" s="121"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="120"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
created a normalized database
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="212">
   <si>
     <t>Задание</t>
   </si>
@@ -213,9 +213,6 @@
     <t>Як користувач, хочу видалити переписку з обох сторін</t>
   </si>
   <si>
-    <t>Як користувач, хочу видалити переписку зі своєї сторони</t>
-  </si>
-  <si>
     <t>Як користувач, хочу відповісти на повідомлення</t>
   </si>
   <si>
@@ -228,22 +225,10 @@
     <t>Як користувач, хочу видалити повідомлення з обох сторін</t>
   </si>
   <si>
-    <t>Як користувач, хочу видалити повідомлення зі своєї сторони</t>
-  </si>
-  <si>
-    <t>Як користувач хочу відповісти на коментар іншого користувача</t>
-  </si>
-  <si>
     <t>Як користувач, хочу вподобати коментар</t>
   </si>
   <si>
     <t>Як користувач, хочу редагувати коментар</t>
-  </si>
-  <si>
-    <t>Як користувач, хочу вподобати фото</t>
-  </si>
-  <si>
-    <t>Як користувач, хочу прокоментувати фото</t>
   </si>
   <si>
     <t>Як користувач, хочу додати фото профіля</t>
@@ -292,9 +277,6 @@
   </si>
   <si>
     <t>Як адміністратор, хочу переглядати статистику</t>
-  </si>
-  <si>
-    <t>Як користувач, хочу знати скільки користувачів переглянули допис</t>
   </si>
   <si>
     <t>Як користувач, хочу мати сповіщення про нові повідомлення</t>
@@ -1204,6 +1186,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1213,76 +1204,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1294,11 +1216,26 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1312,6 +1249,15 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1319,6 +1265,42 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -29069,10 +29051,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1027"/>
+  <dimension ref="A1:AA1021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -29166,7 +29148,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="32" t="s">
@@ -29276,10 +29258,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="32"/>
@@ -29311,7 +29293,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>25</v>
@@ -29455,7 +29437,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>23</v>
@@ -29490,10 +29472,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -29592,13 +29574,13 @@
     </row>
     <row r="15" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="78">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -29627,13 +29609,13 @@
     </row>
     <row r="16" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A16" s="78">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -29662,13 +29644,13 @@
     </row>
     <row r="17" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="78">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>59</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -29697,7 +29679,7 @@
     </row>
     <row r="18" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A18" s="78">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>60</v>
@@ -29732,13 +29714,13 @@
     </row>
     <row r="19" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A19" s="78">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -29767,13 +29749,13 @@
     </row>
     <row r="20" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A20" s="78">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -29802,13 +29784,13 @@
     </row>
     <row r="21" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A21" s="78">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -29835,15 +29817,15 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="22" spans="1:27" ht="15" customHeight="1">
       <c r="A22" s="78">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -29870,15 +29852,15 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="23" spans="1:27" ht="15" customHeight="1">
       <c r="A23" s="78">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -29907,13 +29889,13 @@
     </row>
     <row r="24" spans="1:27" ht="15" customHeight="1">
       <c r="A24" s="78">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -29940,12 +29922,12 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" ht="15" customHeight="1">
+    <row r="25" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A25" s="78">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>24</v>
@@ -29975,15 +29957,15 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" ht="15" customHeight="1">
+    <row r="26" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A26" s="78">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B26" s="34" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -30010,12 +29992,12 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="27" spans="1:27" s="77" customFormat="1" ht="15" customHeight="1">
       <c r="A27" s="78">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B27" s="34" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>24</v>
@@ -30045,12 +30027,12 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="28" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="78">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>24</v>
@@ -30080,12 +30062,12 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="1:27" s="77" customFormat="1" ht="15" customHeight="1">
+    <row r="29" spans="1:27" ht="15" customHeight="1">
       <c r="A29" s="78">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>215</v>
+        <v>65</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>24</v>
@@ -30115,15 +30097,15 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
+    <row r="30" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A30" s="78">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>175</v>
+        <v>110</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -30150,15 +30132,15 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" spans="1:27" ht="15" customHeight="1">
+    <row r="31" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
       <c r="A31" s="78">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -30187,13 +30169,13 @@
     </row>
     <row r="32" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A32" s="78">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -30220,15 +30202,15 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="1:27" s="66" customFormat="1" ht="15" customHeight="1">
+    <row r="33" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
       <c r="A33" s="78">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>178</v>
+        <v>68</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -30255,12 +30237,12 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="34" spans="1:27" ht="14.4" customHeight="1">
       <c r="A34" s="78">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="C34" s="32" t="s">
         <v>24</v>
@@ -30290,12 +30272,12 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="1:27" s="65" customFormat="1" ht="15" customHeight="1">
+    <row r="35" spans="1:27" ht="13.2" customHeight="1">
       <c r="A35" s="78">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="34" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C35" s="32" t="s">
         <v>24</v>
@@ -30325,15 +30307,15 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="1:27" ht="14.4" customHeight="1">
+    <row r="36" spans="1:27" s="65" customFormat="1" ht="13.2" customHeight="1">
       <c r="A36" s="78">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -30360,12 +30342,12 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="1:27" ht="13.2" customHeight="1">
+    <row r="37" spans="1:27" ht="13.8" customHeight="1">
       <c r="A37" s="78">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="32" t="s">
         <v>24</v>
@@ -30395,15 +30377,15 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
     </row>
-    <row r="38" spans="1:27" s="65" customFormat="1" ht="13.2" customHeight="1">
+    <row r="38" spans="1:27" ht="13.2" customHeight="1">
       <c r="A38" s="78">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -30430,15 +30412,15 @@
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
     </row>
-    <row r="39" spans="1:27" s="65" customFormat="1" ht="13.2" customHeight="1">
+    <row r="39" spans="1:27" ht="16.8" customHeight="1">
       <c r="A39" s="78">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B39" s="34" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -30465,15 +30447,15 @@
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
     </row>
-    <row r="40" spans="1:27" ht="13.8" customHeight="1">
+    <row r="40" spans="1:27" ht="16.2" customHeight="1">
       <c r="A40" s="78">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B40" s="34" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -30500,15 +30482,15 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" spans="1:27" ht="15.6" customHeight="1">
+    <row r="41" spans="1:27" s="65" customFormat="1" ht="16.2" customHeight="1">
       <c r="A41" s="78">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B41" s="34" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -30535,15 +30517,15 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
     </row>
-    <row r="42" spans="1:27" ht="13.2" customHeight="1">
+    <row r="42" spans="1:27" ht="13.8" customHeight="1">
       <c r="A42" s="78">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B42" s="34" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -30570,15 +30552,15 @@
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
     </row>
-    <row r="43" spans="1:27" ht="16.8" customHeight="1">
+    <row r="43" spans="1:27" s="77" customFormat="1" ht="13.8" customHeight="1">
       <c r="A43" s="78">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B43" s="34" t="s">
-        <v>66</v>
+        <v>208</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -30605,15 +30587,15 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
     </row>
-    <row r="44" spans="1:27" ht="16.2" customHeight="1">
+    <row r="44" spans="1:27" ht="15" customHeight="1">
       <c r="A44" s="78">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B44" s="34" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -30640,15 +30622,15 @@
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
     </row>
-    <row r="45" spans="1:27" s="65" customFormat="1" ht="16.2" customHeight="1">
+    <row r="45" spans="1:27" ht="13.8" customHeight="1">
       <c r="A45" s="78">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B45" s="34" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -30675,15 +30657,15 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" spans="1:27" ht="13.8" customHeight="1">
+    <row r="46" spans="1:27" ht="16.2" customHeight="1">
       <c r="A46" s="78">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B46" s="34" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -30710,15 +30692,15 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" spans="1:27" ht="13.2" customHeight="1">
+    <row r="47" spans="1:27" ht="13.8">
       <c r="A47" s="78">
-        <v>46</v>
+        <v>52</v>
       </c>
-      <c r="B47" s="34" t="s">
-        <v>68</v>
+      <c r="B47" s="68" t="s">
+        <v>75</v>
       </c>
-      <c r="C47" s="32" t="s">
-        <v>24</v>
+      <c r="C47" s="67" t="s">
+        <v>81</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -30745,15 +30727,15 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" spans="1:27" ht="13.8" customHeight="1">
+    <row r="48" spans="1:27" s="65" customFormat="1" ht="13.8">
       <c r="A48" s="78">
-        <v>47</v>
+        <v>53</v>
       </c>
-      <c r="B48" s="34" t="s">
-        <v>76</v>
+      <c r="B48" s="68" t="s">
+        <v>82</v>
       </c>
-      <c r="C48" s="32" t="s">
-        <v>25</v>
+      <c r="C48" s="67" t="s">
+        <v>83</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -30780,14 +30762,14 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="1:27" s="77" customFormat="1" ht="13.8" customHeight="1">
+    <row r="49" spans="1:27" s="65" customFormat="1" ht="13.8">
       <c r="A49" s="78">
-        <v>48</v>
+        <v>54</v>
       </c>
-      <c r="B49" s="34" t="s">
-        <v>214</v>
+      <c r="B49" s="68" t="s">
+        <v>78</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="69" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="2"/>
@@ -30815,14 +30797,14 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" ht="15" customHeight="1">
+    <row r="50" spans="1:27" s="65" customFormat="1" ht="13.8">
       <c r="A50" s="78">
-        <v>49</v>
+        <v>55</v>
       </c>
-      <c r="B50" s="34" t="s">
-        <v>77</v>
+      <c r="B50" s="68" t="s">
+        <v>88</v>
       </c>
-      <c r="C50" s="32" t="s">
+      <c r="C50" s="69" t="s">
         <v>25</v>
       </c>
       <c r="D50" s="2"/>
@@ -30850,15 +30832,15 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" spans="1:27" ht="13.8" customHeight="1">
+    <row r="51" spans="1:27" s="66" customFormat="1" ht="13.8">
       <c r="A51" s="78">
-        <v>50</v>
+        <v>56</v>
       </c>
-      <c r="B51" s="34" t="s">
-        <v>114</v>
+      <c r="B51" s="68" t="s">
+        <v>206</v>
       </c>
-      <c r="C51" s="32" t="s">
-        <v>25</v>
+      <c r="C51" s="69" t="s">
+        <v>83</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -30885,15 +30867,15 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" spans="1:27" ht="16.2" customHeight="1">
+    <row r="52" spans="1:27" ht="13.8">
       <c r="A52" s="78">
-        <v>51</v>
+        <v>57</v>
       </c>
-      <c r="B52" s="34" t="s">
-        <v>79</v>
+      <c r="B52" s="2" t="s">
+        <v>76</v>
       </c>
-      <c r="C52" s="32" t="s">
-        <v>23</v>
+      <c r="C52" s="69" t="s">
+        <v>83</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -30920,15 +30902,15 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" spans="1:27" ht="13.8">
+    <row r="53" spans="1:27" s="77" customFormat="1" ht="13.8">
       <c r="A53" s="78">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B53" s="68" t="s">
-        <v>80</v>
+        <v>211</v>
       </c>
-      <c r="C53" s="67" t="s">
-        <v>87</v>
+      <c r="C53" s="69" t="s">
+        <v>83</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -30955,15 +30937,15 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="1:27" s="65" customFormat="1" ht="13.8">
+    <row r="54" spans="1:27" s="77" customFormat="1" ht="13.8">
       <c r="A54" s="78">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B54" s="68" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
-      <c r="C54" s="67" t="s">
-        <v>89</v>
+      <c r="C54" s="69" t="s">
+        <v>83</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -30990,15 +30972,15 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="1:27" s="65" customFormat="1" ht="13.8">
+    <row r="55" spans="1:27" ht="13.8">
       <c r="A55" s="78">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B55" s="68" t="s">
-        <v>83</v>
+        <v>210</v>
       </c>
       <c r="C55" s="69" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -31025,15 +31007,15 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="1:27" s="65" customFormat="1" ht="13.8">
+    <row r="56" spans="1:27" ht="13.8">
       <c r="A56" s="78">
-        <v>55</v>
+        <v>61</v>
       </c>
-      <c r="B56" s="68" t="s">
-        <v>94</v>
+      <c r="B56" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="C56" s="69" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -31060,16 +31042,9 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="1:27" s="66" customFormat="1" ht="13.8">
-      <c r="A57" s="78">
-        <v>56</v>
-      </c>
-      <c r="B57" s="68" t="s">
-        <v>212</v>
-      </c>
-      <c r="C57" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="57" spans="1:27" ht="13.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -31095,16 +31070,9 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="1:27" ht="13.8">
-      <c r="A58" s="78">
-        <v>57</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="58" spans="1:27" ht="13.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
@@ -31130,16 +31098,9 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" spans="1:27" s="77" customFormat="1" ht="13.8">
-      <c r="A59" s="78">
-        <v>58</v>
-      </c>
-      <c r="B59" s="68" t="s">
-        <v>217</v>
-      </c>
-      <c r="C59" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="59" spans="1:27" ht="13.2">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
@@ -31165,16 +31126,9 @@
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" spans="1:27" s="77" customFormat="1" ht="13.8">
-      <c r="A60" s="78">
-        <v>59</v>
-      </c>
-      <c r="B60" s="68" t="s">
-        <v>82</v>
-      </c>
-      <c r="C60" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="60" spans="1:27" ht="13.2">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
@@ -31200,16 +31154,9 @@
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" spans="1:27" ht="13.8">
-      <c r="A61" s="78">
-        <v>60</v>
-      </c>
-      <c r="B61" s="68" t="s">
-        <v>216</v>
-      </c>
-      <c r="C61" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="61" spans="1:27" ht="13.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
@@ -31235,16 +31182,9 @@
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" spans="1:27" ht="13.8">
-      <c r="A62" s="78">
-        <v>61</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C62" s="69" t="s">
-        <v>89</v>
-      </c>
+    <row r="62" spans="1:27" ht="13.2">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -58121,174 +58061,6 @@
       <c r="Y1021" s="2"/>
       <c r="Z1021" s="2"/>
       <c r="AA1021" s="2"/>
-    </row>
-    <row r="1022" spans="2:27" ht="13.2">
-      <c r="B1022" s="2"/>
-      <c r="C1022" s="2"/>
-      <c r="D1022" s="2"/>
-      <c r="E1022" s="2"/>
-      <c r="F1022" s="2"/>
-      <c r="G1022" s="2"/>
-      <c r="H1022" s="2"/>
-      <c r="I1022" s="2"/>
-      <c r="J1022" s="2"/>
-      <c r="K1022" s="2"/>
-      <c r="L1022" s="2"/>
-      <c r="M1022" s="2"/>
-      <c r="N1022" s="2"/>
-      <c r="O1022" s="2"/>
-      <c r="P1022" s="2"/>
-      <c r="Q1022" s="2"/>
-      <c r="R1022" s="2"/>
-      <c r="S1022" s="2"/>
-      <c r="T1022" s="2"/>
-      <c r="U1022" s="2"/>
-      <c r="V1022" s="2"/>
-      <c r="W1022" s="2"/>
-      <c r="X1022" s="2"/>
-      <c r="Y1022" s="2"/>
-      <c r="Z1022" s="2"/>
-      <c r="AA1022" s="2"/>
-    </row>
-    <row r="1023" spans="2:27" ht="13.2">
-      <c r="B1023" s="2"/>
-      <c r="C1023" s="2"/>
-      <c r="D1023" s="2"/>
-      <c r="E1023" s="2"/>
-      <c r="F1023" s="2"/>
-      <c r="G1023" s="2"/>
-      <c r="H1023" s="2"/>
-      <c r="I1023" s="2"/>
-      <c r="J1023" s="2"/>
-      <c r="K1023" s="2"/>
-      <c r="L1023" s="2"/>
-      <c r="M1023" s="2"/>
-      <c r="N1023" s="2"/>
-      <c r="O1023" s="2"/>
-      <c r="P1023" s="2"/>
-      <c r="Q1023" s="2"/>
-      <c r="R1023" s="2"/>
-      <c r="S1023" s="2"/>
-      <c r="T1023" s="2"/>
-      <c r="U1023" s="2"/>
-      <c r="V1023" s="2"/>
-      <c r="W1023" s="2"/>
-      <c r="X1023" s="2"/>
-      <c r="Y1023" s="2"/>
-      <c r="Z1023" s="2"/>
-      <c r="AA1023" s="2"/>
-    </row>
-    <row r="1024" spans="2:27" ht="13.2">
-      <c r="B1024" s="2"/>
-      <c r="C1024" s="2"/>
-      <c r="D1024" s="2"/>
-      <c r="E1024" s="2"/>
-      <c r="F1024" s="2"/>
-      <c r="G1024" s="2"/>
-      <c r="H1024" s="2"/>
-      <c r="I1024" s="2"/>
-      <c r="J1024" s="2"/>
-      <c r="K1024" s="2"/>
-      <c r="L1024" s="2"/>
-      <c r="M1024" s="2"/>
-      <c r="N1024" s="2"/>
-      <c r="O1024" s="2"/>
-      <c r="P1024" s="2"/>
-      <c r="Q1024" s="2"/>
-      <c r="R1024" s="2"/>
-      <c r="S1024" s="2"/>
-      <c r="T1024" s="2"/>
-      <c r="U1024" s="2"/>
-      <c r="V1024" s="2"/>
-      <c r="W1024" s="2"/>
-      <c r="X1024" s="2"/>
-      <c r="Y1024" s="2"/>
-      <c r="Z1024" s="2"/>
-      <c r="AA1024" s="2"/>
-    </row>
-    <row r="1025" spans="2:27" ht="13.2">
-      <c r="B1025" s="2"/>
-      <c r="C1025" s="2"/>
-      <c r="D1025" s="2"/>
-      <c r="E1025" s="2"/>
-      <c r="F1025" s="2"/>
-      <c r="G1025" s="2"/>
-      <c r="H1025" s="2"/>
-      <c r="I1025" s="2"/>
-      <c r="J1025" s="2"/>
-      <c r="K1025" s="2"/>
-      <c r="L1025" s="2"/>
-      <c r="M1025" s="2"/>
-      <c r="N1025" s="2"/>
-      <c r="O1025" s="2"/>
-      <c r="P1025" s="2"/>
-      <c r="Q1025" s="2"/>
-      <c r="R1025" s="2"/>
-      <c r="S1025" s="2"/>
-      <c r="T1025" s="2"/>
-      <c r="U1025" s="2"/>
-      <c r="V1025" s="2"/>
-      <c r="W1025" s="2"/>
-      <c r="X1025" s="2"/>
-      <c r="Y1025" s="2"/>
-      <c r="Z1025" s="2"/>
-      <c r="AA1025" s="2"/>
-    </row>
-    <row r="1026" spans="2:27" ht="13.2">
-      <c r="B1026" s="2"/>
-      <c r="C1026" s="2"/>
-      <c r="D1026" s="2"/>
-      <c r="E1026" s="2"/>
-      <c r="F1026" s="2"/>
-      <c r="G1026" s="2"/>
-      <c r="H1026" s="2"/>
-      <c r="I1026" s="2"/>
-      <c r="J1026" s="2"/>
-      <c r="K1026" s="2"/>
-      <c r="L1026" s="2"/>
-      <c r="M1026" s="2"/>
-      <c r="N1026" s="2"/>
-      <c r="O1026" s="2"/>
-      <c r="P1026" s="2"/>
-      <c r="Q1026" s="2"/>
-      <c r="R1026" s="2"/>
-      <c r="S1026" s="2"/>
-      <c r="T1026" s="2"/>
-      <c r="U1026" s="2"/>
-      <c r="V1026" s="2"/>
-      <c r="W1026" s="2"/>
-      <c r="X1026" s="2"/>
-      <c r="Y1026" s="2"/>
-      <c r="Z1026" s="2"/>
-      <c r="AA1026" s="2"/>
-    </row>
-    <row r="1027" spans="2:27" ht="13.2">
-      <c r="B1027" s="2"/>
-      <c r="C1027" s="2"/>
-      <c r="D1027" s="2"/>
-      <c r="E1027" s="2"/>
-      <c r="F1027" s="2"/>
-      <c r="G1027" s="2"/>
-      <c r="H1027" s="2"/>
-      <c r="I1027" s="2"/>
-      <c r="J1027" s="2"/>
-      <c r="K1027" s="2"/>
-      <c r="L1027" s="2"/>
-      <c r="M1027" s="2"/>
-      <c r="N1027" s="2"/>
-      <c r="O1027" s="2"/>
-      <c r="P1027" s="2"/>
-      <c r="Q1027" s="2"/>
-      <c r="R1027" s="2"/>
-      <c r="S1027" s="2"/>
-      <c r="T1027" s="2"/>
-      <c r="U1027" s="2"/>
-      <c r="V1027" s="2"/>
-      <c r="W1027" s="2"/>
-      <c r="X1027" s="2"/>
-      <c r="Y1027" s="2"/>
-      <c r="Z1027" s="2"/>
-      <c r="AA1027" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -58410,13 +58182,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="79" t="s">
+      <c r="B6" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="115" t="s">
+      <c r="C6" s="103" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="42" t="s">
@@ -58425,14 +58197,14 @@
       <c r="E6" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="79" t="s">
+      <c r="F6" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="49"/>
-      <c r="H6" s="115">
+      <c r="H6" s="103">
         <v>4</v>
       </c>
-      <c r="I6" s="87">
+      <c r="I6" s="93">
         <v>7</v>
       </c>
       <c r="J6" s="39">
@@ -58440,83 +58212,83 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A7" s="104"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="116"/>
+      <c r="A7" s="85"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="42" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
-      <c r="F7" s="80"/>
+      <c r="F7" s="83"/>
       <c r="G7" s="50"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="89"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="94"/>
       <c r="J7" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="39" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A8" s="104"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="116"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="57" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="83"/>
       <c r="G8" s="56"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="89"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="94"/>
       <c r="J8" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A9" s="105"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="117"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="105"/>
       <c r="D9" s="45" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="50"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="88"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="95"/>
       <c r="J9" s="75">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="82" t="s">
-        <v>213</v>
+      <c r="C10" s="79" t="s">
+        <v>207</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E10" s="62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="49"/>
-      <c r="H10" s="85">
+      <c r="H10" s="100">
         <v>4</v>
       </c>
-      <c r="I10" s="87">
+      <c r="I10" s="93">
         <v>8</v>
       </c>
       <c r="J10" s="75">
@@ -58524,101 +58296,101 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A11" s="104"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="83"/>
+      <c r="A11" s="85"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="71" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E11" s="62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
-      <c r="F11" s="80"/>
+      <c r="F11" s="83"/>
       <c r="G11" s="49"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="89"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A12" s="104"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="83"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="80"/>
       <c r="D12" s="71" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E12" s="62" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
-      <c r="F12" s="80"/>
+      <c r="F12" s="83"/>
       <c r="G12" s="49"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="89"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="94"/>
       <c r="J12" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A13" s="104"/>
-      <c r="B13" s="80"/>
-      <c r="C13" s="83"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="80"/>
       <c r="D13" s="71" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E13" s="62" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
-      <c r="F13" s="80"/>
+      <c r="F13" s="83"/>
       <c r="G13" s="50"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="89"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="94"/>
       <c r="J13" s="75">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="55" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A14" s="105"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="84"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="59" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E14" s="72" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
-      <c r="F14" s="81"/>
+      <c r="F14" s="84"/>
       <c r="G14" s="70"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="88"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="95"/>
       <c r="J14" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A15" s="112" t="s">
+      <c r="A15" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="82" t="s">
-        <v>98</v>
+      <c r="C15" s="79" t="s">
+        <v>92</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
-      <c r="F15" s="79" t="s">
+      <c r="F15" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="49"/>
-      <c r="H15" s="85">
+      <c r="H15" s="100">
         <v>3</v>
       </c>
-      <c r="I15" s="87">
+      <c r="I15" s="93">
         <v>6</v>
       </c>
       <c r="J15" s="66">
@@ -58626,83 +58398,83 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A16" s="113"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="83"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="62" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E16" s="73" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
-      <c r="F16" s="80"/>
+      <c r="F16" s="83"/>
       <c r="G16" s="50"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="89"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="94"/>
       <c r="J16" s="66">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A17" s="113"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="83"/>
+      <c r="A17" s="98"/>
+      <c r="B17" s="83"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="62" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E17" s="73" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
-      <c r="F17" s="80"/>
+      <c r="F17" s="83"/>
       <c r="G17" s="50"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="89"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="94"/>
       <c r="J17" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A18" s="114"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="84"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="48" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E18" s="73" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="84"/>
       <c r="G18" s="50"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="88"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="95"/>
       <c r="J18" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A19" s="104" t="s">
-        <v>132</v>
+      <c r="A19" s="85" t="s">
+        <v>126</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="82" t="s">
-        <v>120</v>
+      <c r="C19" s="79" t="s">
+        <v>114</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E19" s="72" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
-      <c r="F19" s="79" t="s">
+      <c r="F19" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G19" s="70"/>
-      <c r="H19" s="85">
+      <c r="H19" s="100">
         <v>2</v>
       </c>
-      <c r="I19" s="87">
+      <c r="I19" s="93">
         <v>3</v>
       </c>
       <c r="J19" s="66">
@@ -58710,47 +58482,47 @@
       </c>
     </row>
     <row r="20" spans="1:27" s="65" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A20" s="104"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="83"/>
+      <c r="A20" s="85"/>
+      <c r="B20" s="83"/>
+      <c r="C20" s="80"/>
       <c r="D20" s="54" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E20" s="72" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
-      <c r="F20" s="81"/>
+      <c r="F20" s="84"/>
       <c r="G20" s="70"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="88"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="95"/>
       <c r="J20" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="82" t="s">
-        <v>91</v>
+      <c r="C21" s="79" t="s">
+        <v>85</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E21" s="47" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
-      <c r="F21" s="79" t="s">
+      <c r="F21" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="49"/>
-      <c r="H21" s="85">
+      <c r="H21" s="100">
         <v>3</v>
       </c>
-      <c r="I21" s="87">
+      <c r="I21" s="93">
         <v>5</v>
       </c>
       <c r="J21" s="66">
@@ -58758,63 +58530,63 @@
       </c>
     </row>
     <row r="22" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A22" s="104"/>
-      <c r="B22" s="80"/>
-      <c r="C22" s="83"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="80"/>
       <c r="D22" s="47" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
-      <c r="E22" s="101" t="s">
-        <v>138</v>
+      <c r="E22" s="91" t="s">
+        <v>132</v>
       </c>
-      <c r="F22" s="80"/>
+      <c r="F22" s="83"/>
       <c r="G22" s="49"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="89"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="94"/>
       <c r="J22" s="66">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="16.5" customHeight="1">
-      <c r="A23" s="104"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="81"/>
       <c r="D23" s="62" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
-      <c r="E23" s="111"/>
-      <c r="F23" s="81"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="84"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="88"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="95"/>
       <c r="J23" s="66">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A24" s="103" t="s">
-        <v>140</v>
+      <c r="A24" s="89" t="s">
+        <v>134</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="82" t="s">
-        <v>139</v>
+      <c r="C24" s="79" t="s">
+        <v>133</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
-      <c r="E24" s="106" t="s">
-        <v>152</v>
+      <c r="E24" s="86" t="s">
+        <v>146</v>
       </c>
-      <c r="F24" s="79" t="s">
+      <c r="F24" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G24" s="49"/>
-      <c r="H24" s="85">
+      <c r="H24" s="100">
         <v>3</v>
       </c>
-      <c r="I24" s="87">
+      <c r="I24" s="93">
         <v>5</v>
       </c>
       <c r="J24" s="76">
@@ -58839,17 +58611,17 @@
       <c r="AA24" s="18"/>
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A25" s="104"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="83"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="80"/>
       <c r="D25" s="72" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
-      <c r="E25" s="107"/>
-      <c r="F25" s="80"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="83"/>
       <c r="G25" s="50"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="89"/>
+      <c r="H25" s="101"/>
+      <c r="I25" s="94"/>
       <c r="J25" s="76">
         <v>2</v>
       </c>
@@ -58872,17 +58644,17 @@
       <c r="AA25" s="18"/>
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A26" s="105"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="84"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="62" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
-      <c r="E26" s="108"/>
-      <c r="F26" s="81"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="84"/>
       <c r="G26" s="51"/>
-      <c r="H26" s="86"/>
-      <c r="I26" s="88"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="95"/>
       <c r="J26" s="76">
         <v>2</v>
       </c>
@@ -58905,27 +58677,27 @@
       <c r="AA26" s="18"/>
     </row>
     <row r="27" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A27" s="103" t="s">
-        <v>95</v>
+      <c r="A27" s="89" t="s">
+        <v>89</v>
       </c>
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="82" t="s">
-        <v>144</v>
+      <c r="C27" s="79" t="s">
+        <v>138</v>
       </c>
       <c r="D27" s="54" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
-      <c r="E27" s="106" t="s">
-        <v>153</v>
+      <c r="E27" s="86" t="s">
+        <v>147</v>
       </c>
       <c r="F27" s="63"/>
       <c r="G27" s="70"/>
-      <c r="H27" s="90">
+      <c r="H27" s="111">
         <v>2</v>
       </c>
-      <c r="I27" s="87">
+      <c r="I27" s="93">
         <v>4</v>
       </c>
       <c r="J27" s="76">
@@ -58950,19 +58722,19 @@
       <c r="AA27" s="18"/>
     </row>
     <row r="28" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A28" s="104"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="83"/>
+      <c r="A28" s="85"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="80"/>
       <c r="D28" s="36" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
-      <c r="E28" s="107"/>
+      <c r="E28" s="87"/>
       <c r="F28" s="63" t="s">
         <v>39</v>
       </c>
       <c r="G28" s="70"/>
-      <c r="H28" s="91"/>
-      <c r="I28" s="89"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="94"/>
       <c r="J28" s="76">
         <v>1</v>
       </c>
@@ -58985,17 +58757,17 @@
       <c r="AA28" s="18"/>
     </row>
     <row r="29" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A29" s="105"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="84"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="81"/>
       <c r="D29" s="54" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
-      <c r="E29" s="108"/>
+      <c r="E29" s="88"/>
       <c r="F29" s="63"/>
       <c r="G29" s="70"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="88"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="95"/>
       <c r="J29" s="76">
         <v>2</v>
       </c>
@@ -59018,29 +58790,29 @@
       <c r="AA29" s="18"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A30" s="103" t="s">
-        <v>156</v>
+      <c r="A30" s="89" t="s">
+        <v>150</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="82" t="s">
-        <v>93</v>
+      <c r="C30" s="79" t="s">
+        <v>87</v>
       </c>
       <c r="D30" s="37" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
-      <c r="E30" s="101" t="s">
-        <v>155</v>
+      <c r="E30" s="91" t="s">
+        <v>149</v>
       </c>
-      <c r="F30" s="79" t="s">
+      <c r="F30" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G30" s="49"/>
-      <c r="H30" s="85">
+      <c r="H30" s="100">
         <v>2</v>
       </c>
-      <c r="I30" s="87">
+      <c r="I30" s="93">
         <v>3</v>
       </c>
       <c r="J30" s="76">
@@ -59065,17 +58837,17 @@
       <c r="AA30" s="18"/>
     </row>
     <row r="31" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A31" s="104"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="83"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="80"/>
       <c r="D31" s="74" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
-      <c r="E31" s="102"/>
-      <c r="F31" s="80"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="83"/>
       <c r="G31" s="49"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="89"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="94"/>
       <c r="J31" s="76">
         <v>1</v>
       </c>
@@ -59098,17 +58870,17 @@
       <c r="AA31" s="18"/>
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A32" s="104"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="83"/>
+      <c r="A32" s="85"/>
+      <c r="B32" s="83"/>
+      <c r="C32" s="80"/>
       <c r="D32" s="60" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
-      <c r="E32" s="102"/>
-      <c r="F32" s="81"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="84"/>
       <c r="G32" s="64"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="89"/>
+      <c r="H32" s="101"/>
+      <c r="I32" s="94"/>
       <c r="J32" s="76">
         <v>1</v>
       </c>
@@ -59131,29 +58903,29 @@
       <c r="AA32" s="18"/>
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A33" s="103" t="s">
-        <v>158</v>
+      <c r="A33" s="89" t="s">
+        <v>152</v>
       </c>
-      <c r="B33" s="79" t="s">
+      <c r="B33" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="82" t="s">
-        <v>92</v>
+      <c r="C33" s="79" t="s">
+        <v>86</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
-      <c r="E33" s="106" t="s">
-        <v>160</v>
+      <c r="E33" s="86" t="s">
+        <v>154</v>
       </c>
-      <c r="F33" s="79" t="s">
+      <c r="F33" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G33" s="49"/>
-      <c r="H33" s="85">
+      <c r="H33" s="100">
         <v>2</v>
       </c>
-      <c r="I33" s="87">
+      <c r="I33" s="93">
         <v>3</v>
       </c>
       <c r="J33" s="76">
@@ -59178,17 +58950,17 @@
       <c r="AA33" s="18"/>
     </row>
     <row r="34" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A34" s="104"/>
-      <c r="B34" s="80"/>
-      <c r="C34" s="83"/>
+      <c r="A34" s="85"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="80"/>
       <c r="D34" s="74" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
-      <c r="E34" s="107"/>
-      <c r="F34" s="80"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="83"/>
       <c r="G34" s="49"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="89"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="94"/>
       <c r="J34" s="76">
         <v>1</v>
       </c>
@@ -59211,17 +58983,17 @@
       <c r="AA34" s="18"/>
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A35" s="104"/>
-      <c r="B35" s="80"/>
-      <c r="C35" s="83"/>
+      <c r="A35" s="85"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="80"/>
       <c r="D35" s="47" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
-      <c r="E35" s="107"/>
-      <c r="F35" s="80"/>
+      <c r="E35" s="87"/>
+      <c r="F35" s="83"/>
       <c r="G35" s="64"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="89"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="94"/>
       <c r="J35" s="76">
         <v>1</v>
       </c>
@@ -59244,29 +59016,29 @@
       <c r="AA35" s="18"/>
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A36" s="103" t="s">
-        <v>90</v>
+      <c r="A36" s="89" t="s">
+        <v>84</v>
       </c>
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="79" t="s">
         <v>48</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
-      <c r="E36" s="106" t="s">
-        <v>166</v>
+      <c r="E36" s="86" t="s">
+        <v>160</v>
       </c>
-      <c r="F36" s="79" t="s">
+      <c r="F36" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G36" s="49"/>
-      <c r="H36" s="97">
+      <c r="H36" s="114">
         <v>4</v>
       </c>
-      <c r="I36" s="87">
+      <c r="I36" s="93">
         <v>8</v>
       </c>
       <c r="J36" s="76">
@@ -59291,17 +59063,17 @@
       <c r="AA36" s="18"/>
     </row>
     <row r="37" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A37" s="104"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="83"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="80"/>
       <c r="D37" s="37" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
-      <c r="E37" s="107"/>
-      <c r="F37" s="80"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="83"/>
       <c r="G37" s="49"/>
-      <c r="H37" s="98"/>
-      <c r="I37" s="89"/>
+      <c r="H37" s="115"/>
+      <c r="I37" s="94"/>
       <c r="J37" s="76">
         <v>1</v>
       </c>
@@ -59324,17 +59096,17 @@
       <c r="AA37" s="18"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A38" s="104"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="83"/>
+      <c r="A38" s="85"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="80"/>
       <c r="D38" s="62" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
-      <c r="E38" s="107"/>
-      <c r="F38" s="80"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="83"/>
       <c r="G38" s="50"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="89"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="94"/>
       <c r="J38" s="76">
         <v>1</v>
       </c>
@@ -59357,17 +59129,17 @@
       <c r="AA38" s="18"/>
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A39" s="105"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="84"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="84"/>
+      <c r="C39" s="81"/>
       <c r="D39" s="61" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
-      <c r="E39" s="108"/>
-      <c r="F39" s="81"/>
+      <c r="E39" s="88"/>
+      <c r="F39" s="84"/>
       <c r="G39" s="51"/>
-      <c r="H39" s="100"/>
-      <c r="I39" s="88"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="95"/>
       <c r="J39" s="76">
         <v>5</v>
       </c>
@@ -59390,29 +59162,29 @@
       <c r="AA39" s="18"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A40" s="103" t="s">
-        <v>60</v>
+      <c r="A40" s="89" t="s">
+        <v>59</v>
       </c>
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="82" t="s">
-        <v>96</v>
+      <c r="C40" s="79" t="s">
+        <v>90</v>
       </c>
       <c r="D40" s="37" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E40" s="109" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
-      <c r="F40" s="79" t="s">
+      <c r="F40" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G40" s="49"/>
-      <c r="H40" s="85">
+      <c r="H40" s="100">
         <v>2</v>
       </c>
-      <c r="I40" s="87">
+      <c r="I40" s="93">
         <v>3</v>
       </c>
       <c r="J40" s="76">
@@ -59437,17 +59209,17 @@
       <c r="AA40" s="18"/>
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A41" s="104"/>
-      <c r="B41" s="80"/>
-      <c r="C41" s="83"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="80"/>
       <c r="D41" s="47" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E41" s="110"/>
-      <c r="F41" s="80"/>
+      <c r="F41" s="83"/>
       <c r="G41" s="64"/>
-      <c r="H41" s="93"/>
-      <c r="I41" s="89"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="94"/>
       <c r="J41" s="76">
         <v>1</v>
       </c>
@@ -59470,29 +59242,29 @@
       <c r="AA41" s="18"/>
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A42" s="103" t="s">
-        <v>61</v>
+      <c r="A42" s="89" t="s">
+        <v>60</v>
       </c>
-      <c r="B42" s="79" t="s">
+      <c r="B42" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="82" t="s">
-        <v>97</v>
+      <c r="C42" s="79" t="s">
+        <v>91</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
-      <c r="E42" s="101" t="s">
-        <v>169</v>
+      <c r="E42" s="91" t="s">
+        <v>163</v>
       </c>
-      <c r="F42" s="79" t="s">
+      <c r="F42" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="49"/>
-      <c r="H42" s="85">
+      <c r="H42" s="100">
         <v>2</v>
       </c>
-      <c r="I42" s="87">
+      <c r="I42" s="93">
         <v>3</v>
       </c>
       <c r="J42" s="76">
@@ -59517,17 +59289,17 @@
       <c r="AA42" s="18"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A43" s="104"/>
-      <c r="B43" s="80"/>
-      <c r="C43" s="83"/>
+      <c r="A43" s="85"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="80"/>
       <c r="D43" s="37" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
-      <c r="E43" s="102"/>
-      <c r="F43" s="81"/>
+      <c r="E43" s="92"/>
+      <c r="F43" s="84"/>
       <c r="G43" s="64"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="89"/>
+      <c r="H43" s="101"/>
+      <c r="I43" s="94"/>
       <c r="J43" s="76">
         <v>1</v>
       </c>
@@ -59550,29 +59322,29 @@
       <c r="AA43" s="18"/>
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A44" s="103" t="s">
-        <v>172</v>
+      <c r="A44" s="89" t="s">
+        <v>166</v>
       </c>
-      <c r="B44" s="79" t="s">
+      <c r="B44" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="82" t="s">
-        <v>176</v>
+      <c r="C44" s="79" t="s">
+        <v>170</v>
       </c>
       <c r="D44" s="60" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
-      <c r="E44" s="101" t="s">
-        <v>193</v>
+      <c r="E44" s="91" t="s">
+        <v>187</v>
       </c>
-      <c r="F44" s="79" t="s">
+      <c r="F44" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="50"/>
-      <c r="H44" s="85">
+      <c r="H44" s="100">
         <v>2</v>
       </c>
-      <c r="I44" s="87">
+      <c r="I44" s="93">
         <v>4</v>
       </c>
       <c r="J44" s="76">
@@ -59597,17 +59369,17 @@
       <c r="AA44" s="18"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A45" s="104"/>
-      <c r="B45" s="80"/>
-      <c r="C45" s="83"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="80"/>
       <c r="D45" s="73" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
-      <c r="E45" s="102"/>
-      <c r="F45" s="80"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="83"/>
       <c r="G45" s="56"/>
-      <c r="H45" s="93"/>
-      <c r="I45" s="89"/>
+      <c r="H45" s="101"/>
+      <c r="I45" s="94"/>
       <c r="J45" s="76">
         <v>2</v>
       </c>
@@ -59630,29 +59402,29 @@
       <c r="AA45" s="18"/>
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A46" s="103" t="s">
-        <v>116</v>
+      <c r="A46" s="89" t="s">
+        <v>110</v>
       </c>
-      <c r="B46" s="79" t="s">
+      <c r="B46" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="82" t="s">
-        <v>177</v>
+      <c r="C46" s="79" t="s">
+        <v>171</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
-      <c r="E46" s="94" t="s">
-        <v>192</v>
+      <c r="E46" s="106" t="s">
+        <v>186</v>
       </c>
-      <c r="F46" s="79" t="s">
+      <c r="F46" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G46" s="49"/>
-      <c r="H46" s="85">
+      <c r="H46" s="100">
         <v>3</v>
       </c>
-      <c r="I46" s="87">
+      <c r="I46" s="93">
         <v>5</v>
       </c>
       <c r="J46" s="76">
@@ -59677,17 +59449,17 @@
       <c r="AA46" s="18"/>
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A47" s="104"/>
-      <c r="B47" s="80"/>
-      <c r="C47" s="83"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="80"/>
       <c r="D47" s="62" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
-      <c r="E47" s="95"/>
-      <c r="F47" s="80"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="83"/>
       <c r="G47" s="50"/>
-      <c r="H47" s="93"/>
-      <c r="I47" s="89"/>
+      <c r="H47" s="101"/>
+      <c r="I47" s="94"/>
       <c r="J47" s="76">
         <v>2</v>
       </c>
@@ -59710,17 +59482,17 @@
       <c r="AA47" s="18"/>
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A48" s="105"/>
-      <c r="B48" s="81"/>
-      <c r="C48" s="84"/>
+      <c r="A48" s="90"/>
+      <c r="B48" s="84"/>
+      <c r="C48" s="81"/>
       <c r="D48" s="61" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
-      <c r="E48" s="96"/>
-      <c r="F48" s="81"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="84"/>
       <c r="G48" s="51"/>
-      <c r="H48" s="86"/>
-      <c r="I48" s="88"/>
+      <c r="H48" s="102"/>
+      <c r="I48" s="95"/>
       <c r="J48" s="76">
         <v>1</v>
       </c>
@@ -59743,29 +59515,29 @@
       <c r="AA48" s="18"/>
     </row>
     <row r="49" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A49" s="103" t="s">
-        <v>178</v>
+      <c r="A49" s="89" t="s">
+        <v>172</v>
       </c>
-      <c r="B49" s="79" t="s">
+      <c r="B49" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="82" t="s">
-        <v>179</v>
+      <c r="C49" s="79" t="s">
+        <v>173</v>
       </c>
       <c r="D49" s="54" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
-      <c r="E49" s="94" t="s">
-        <v>183</v>
+      <c r="E49" s="106" t="s">
+        <v>177</v>
       </c>
-      <c r="F49" s="79" t="s">
+      <c r="F49" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G49" s="70"/>
-      <c r="H49" s="85">
+      <c r="H49" s="100">
         <v>3</v>
       </c>
-      <c r="I49" s="87">
+      <c r="I49" s="93">
         <v>6</v>
       </c>
       <c r="J49" s="76">
@@ -59790,17 +59562,17 @@
       <c r="AA49" s="18"/>
     </row>
     <row r="50" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A50" s="104"/>
-      <c r="B50" s="80"/>
-      <c r="C50" s="83"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="83"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="54" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
-      <c r="E50" s="95"/>
-      <c r="F50" s="80"/>
+      <c r="E50" s="107"/>
+      <c r="F50" s="83"/>
       <c r="G50" s="70"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="89"/>
+      <c r="H50" s="101"/>
+      <c r="I50" s="94"/>
       <c r="J50" s="76">
         <v>1</v>
       </c>
@@ -59823,17 +59595,17 @@
       <c r="AA50" s="18"/>
     </row>
     <row r="51" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A51" s="105"/>
-      <c r="B51" s="81"/>
-      <c r="C51" s="84"/>
+      <c r="A51" s="90"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="81"/>
       <c r="D51" s="36" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
-      <c r="E51" s="96"/>
-      <c r="F51" s="81"/>
+      <c r="E51" s="108"/>
+      <c r="F51" s="84"/>
       <c r="G51" s="70"/>
-      <c r="H51" s="86"/>
-      <c r="I51" s="88"/>
+      <c r="H51" s="102"/>
+      <c r="I51" s="95"/>
       <c r="J51" s="76">
         <v>4</v>
       </c>
@@ -59856,29 +59628,29 @@
       <c r="AA51" s="18"/>
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A52" s="103" t="s">
-        <v>69</v>
+      <c r="A52" s="89" t="s">
+        <v>64</v>
       </c>
-      <c r="B52" s="79" t="s">
+      <c r="B52" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="82" t="s">
-        <v>194</v>
+      <c r="C52" s="79" t="s">
+        <v>188</v>
       </c>
       <c r="D52" s="37" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
-      <c r="E52" s="94" t="s">
-        <v>187</v>
+      <c r="E52" s="106" t="s">
+        <v>181</v>
       </c>
-      <c r="F52" s="79" t="s">
+      <c r="F52" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G52" s="49"/>
-      <c r="H52" s="85">
+      <c r="H52" s="100">
         <v>2</v>
       </c>
-      <c r="I52" s="87">
+      <c r="I52" s="93">
         <v>4</v>
       </c>
       <c r="J52" s="76">
@@ -59903,17 +59675,17 @@
       <c r="AA52" s="18"/>
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A53" s="104"/>
-      <c r="B53" s="80"/>
-      <c r="C53" s="83"/>
+      <c r="A53" s="85"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="80"/>
       <c r="D53" s="62" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
-      <c r="E53" s="95"/>
-      <c r="F53" s="80"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="83"/>
       <c r="G53" s="50"/>
-      <c r="H53" s="93"/>
-      <c r="I53" s="89"/>
+      <c r="H53" s="101"/>
+      <c r="I53" s="94"/>
       <c r="J53" s="76">
         <v>1</v>
       </c>
@@ -59936,17 +59708,17 @@
       <c r="AA53" s="18"/>
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A54" s="105"/>
-      <c r="B54" s="81"/>
-      <c r="C54" s="84"/>
+      <c r="A54" s="90"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="81"/>
       <c r="D54" s="62" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
-      <c r="E54" s="96"/>
-      <c r="F54" s="81"/>
+      <c r="E54" s="108"/>
+      <c r="F54" s="84"/>
       <c r="G54" s="51"/>
-      <c r="H54" s="86"/>
-      <c r="I54" s="88"/>
+      <c r="H54" s="102"/>
+      <c r="I54" s="95"/>
       <c r="J54" s="76">
         <v>2</v>
       </c>
@@ -59969,27 +59741,27 @@
       <c r="AA54" s="18"/>
     </row>
     <row r="55" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A55" s="103" t="s">
-        <v>118</v>
+      <c r="A55" s="89" t="s">
+        <v>112</v>
       </c>
       <c r="B55" s="63"/>
-      <c r="C55" s="82" t="s">
-        <v>195</v>
+      <c r="C55" s="79" t="s">
+        <v>189</v>
       </c>
       <c r="D55" s="54" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
-      <c r="E55" s="94" t="s">
-        <v>198</v>
+      <c r="E55" s="106" t="s">
+        <v>192</v>
       </c>
-      <c r="F55" s="79" t="s">
+      <c r="F55" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G55" s="70"/>
-      <c r="H55" s="85">
+      <c r="H55" s="100">
         <v>2</v>
       </c>
-      <c r="I55" s="87">
+      <c r="I55" s="93">
         <v>3</v>
       </c>
       <c r="J55" s="76">
@@ -60014,19 +59786,19 @@
       <c r="AA55" s="18"/>
     </row>
     <row r="56" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A56" s="104"/>
+      <c r="A56" s="85"/>
       <c r="B56" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="83"/>
+      <c r="C56" s="80"/>
       <c r="D56" s="54" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
-      <c r="E56" s="95"/>
-      <c r="F56" s="80"/>
+      <c r="E56" s="107"/>
+      <c r="F56" s="83"/>
       <c r="G56" s="70"/>
-      <c r="H56" s="93"/>
-      <c r="I56" s="89"/>
+      <c r="H56" s="101"/>
+      <c r="I56" s="94"/>
       <c r="J56" s="76">
         <v>1</v>
       </c>
@@ -60049,17 +59821,17 @@
       <c r="AA56" s="18"/>
     </row>
     <row r="57" spans="1:27" s="65" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A57" s="105"/>
+      <c r="A57" s="90"/>
       <c r="B57" s="63"/>
-      <c r="C57" s="84"/>
+      <c r="C57" s="81"/>
       <c r="D57" s="54" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
-      <c r="E57" s="96"/>
-      <c r="F57" s="81"/>
+      <c r="E57" s="108"/>
+      <c r="F57" s="84"/>
       <c r="G57" s="70"/>
-      <c r="H57" s="86"/>
-      <c r="I57" s="88"/>
+      <c r="H57" s="102"/>
+      <c r="I57" s="95"/>
       <c r="J57" s="76">
         <v>1</v>
       </c>
@@ -60082,29 +59854,29 @@
       <c r="AA57" s="18"/>
     </row>
     <row r="58" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A58" s="103" t="s">
-        <v>79</v>
+      <c r="A58" s="89" t="s">
+        <v>74</v>
       </c>
-      <c r="B58" s="79" t="s">
+      <c r="B58" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C58" s="82" t="s">
-        <v>99</v>
+      <c r="C58" s="79" t="s">
+        <v>93</v>
       </c>
       <c r="D58" s="37" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
-      <c r="E58" s="94" t="s">
-        <v>202</v>
+      <c r="E58" s="106" t="s">
+        <v>196</v>
       </c>
-      <c r="F58" s="79" t="s">
+      <c r="F58" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G58" s="50"/>
-      <c r="H58" s="85">
+      <c r="H58" s="100">
         <v>2</v>
       </c>
-      <c r="I58" s="87">
+      <c r="I58" s="93">
         <v>4</v>
       </c>
       <c r="J58" s="76">
@@ -60129,17 +59901,17 @@
       <c r="AA58" s="18"/>
     </row>
     <row r="59" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A59" s="104"/>
-      <c r="B59" s="80"/>
-      <c r="C59" s="83"/>
+      <c r="A59" s="85"/>
+      <c r="B59" s="83"/>
+      <c r="C59" s="80"/>
       <c r="D59" s="36" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
-      <c r="E59" s="95"/>
-      <c r="F59" s="80"/>
+      <c r="E59" s="107"/>
+      <c r="F59" s="83"/>
       <c r="G59" s="50"/>
-      <c r="H59" s="93"/>
-      <c r="I59" s="89"/>
+      <c r="H59" s="101"/>
+      <c r="I59" s="94"/>
       <c r="J59" s="76">
         <v>2</v>
       </c>
@@ -60162,17 +59934,17 @@
       <c r="AA59" s="18"/>
     </row>
     <row r="60" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A60" s="105"/>
-      <c r="B60" s="81"/>
-      <c r="C60" s="84"/>
+      <c r="A60" s="90"/>
+      <c r="B60" s="84"/>
+      <c r="C60" s="81"/>
       <c r="D60" s="61" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
-      <c r="E60" s="96"/>
-      <c r="F60" s="81"/>
+      <c r="E60" s="108"/>
+      <c r="F60" s="84"/>
       <c r="G60" s="70"/>
-      <c r="H60" s="86"/>
-      <c r="I60" s="88"/>
+      <c r="H60" s="102"/>
+      <c r="I60" s="95"/>
       <c r="J60" s="76">
         <v>1</v>
       </c>
@@ -60195,29 +59967,29 @@
       <c r="AA60" s="18"/>
     </row>
     <row r="61" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A61" s="103" t="s">
-        <v>80</v>
+      <c r="A61" s="89" t="s">
+        <v>75</v>
       </c>
-      <c r="B61" s="79" t="s">
+      <c r="B61" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C61" s="82" t="s">
-        <v>100</v>
+      <c r="C61" s="79" t="s">
+        <v>94</v>
       </c>
       <c r="D61" s="37" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
-      <c r="E61" s="94" t="s">
-        <v>207</v>
+      <c r="E61" s="106" t="s">
+        <v>201</v>
       </c>
-      <c r="F61" s="79" t="s">
+      <c r="F61" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G61" s="49"/>
-      <c r="H61" s="85">
+      <c r="H61" s="100">
         <v>2</v>
       </c>
-      <c r="I61" s="87">
+      <c r="I61" s="93">
         <v>4</v>
       </c>
       <c r="J61" s="76">
@@ -60242,17 +60014,17 @@
       <c r="AA61" s="18"/>
     </row>
     <row r="62" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A62" s="104"/>
-      <c r="B62" s="80"/>
-      <c r="C62" s="83"/>
+      <c r="A62" s="85"/>
+      <c r="B62" s="83"/>
+      <c r="C62" s="80"/>
       <c r="D62" s="73" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
-      <c r="E62" s="95"/>
-      <c r="F62" s="80"/>
+      <c r="E62" s="107"/>
+      <c r="F62" s="83"/>
       <c r="G62" s="50"/>
-      <c r="H62" s="93"/>
-      <c r="I62" s="89"/>
+      <c r="H62" s="101"/>
+      <c r="I62" s="94"/>
       <c r="J62" s="76">
         <v>1</v>
       </c>
@@ -60275,17 +60047,17 @@
       <c r="AA62" s="18"/>
     </row>
     <row r="63" spans="1:27" s="66" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A63" s="104"/>
-      <c r="B63" s="80"/>
-      <c r="C63" s="83"/>
+      <c r="A63" s="85"/>
+      <c r="B63" s="83"/>
+      <c r="C63" s="80"/>
       <c r="D63" s="73" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
-      <c r="E63" s="95"/>
-      <c r="F63" s="80"/>
+      <c r="E63" s="107"/>
+      <c r="F63" s="83"/>
       <c r="G63" s="50"/>
-      <c r="H63" s="93"/>
-      <c r="I63" s="89"/>
+      <c r="H63" s="101"/>
+      <c r="I63" s="94"/>
       <c r="J63" s="76">
         <v>1</v>
       </c>
@@ -60308,17 +60080,17 @@
       <c r="AA63" s="18"/>
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A64" s="105"/>
-      <c r="B64" s="81"/>
-      <c r="C64" s="84"/>
+      <c r="A64" s="90"/>
+      <c r="B64" s="84"/>
+      <c r="C64" s="81"/>
       <c r="D64" s="62" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
-      <c r="E64" s="96"/>
-      <c r="F64" s="81"/>
+      <c r="E64" s="108"/>
+      <c r="F64" s="84"/>
       <c r="G64" s="50"/>
-      <c r="H64" s="86"/>
-      <c r="I64" s="88"/>
+      <c r="H64" s="102"/>
+      <c r="I64" s="95"/>
       <c r="J64" s="76">
         <v>1</v>
       </c>
@@ -60341,29 +60113,29 @@
       <c r="AA64" s="18"/>
     </row>
     <row r="65" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A65" s="103" t="s">
-        <v>88</v>
+      <c r="A65" s="89" t="s">
+        <v>82</v>
       </c>
-      <c r="B65" s="79" t="s">
+      <c r="B65" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="82" t="s">
-        <v>101</v>
+      <c r="C65" s="79" t="s">
+        <v>95</v>
       </c>
       <c r="D65" s="54" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
-      <c r="E65" s="94" t="s">
-        <v>211</v>
+      <c r="E65" s="106" t="s">
+        <v>205</v>
       </c>
-      <c r="F65" s="79" t="s">
+      <c r="F65" s="82" t="s">
         <v>39</v>
       </c>
       <c r="G65" s="70"/>
-      <c r="H65" s="85">
+      <c r="H65" s="100">
         <v>2</v>
       </c>
-      <c r="I65" s="87">
+      <c r="I65" s="93">
         <v>3</v>
       </c>
       <c r="J65" s="76">
@@ -60388,17 +60160,17 @@
       <c r="AA65" s="18"/>
     </row>
     <row r="66" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A66" s="104"/>
-      <c r="B66" s="80"/>
-      <c r="C66" s="83"/>
+      <c r="A66" s="85"/>
+      <c r="B66" s="83"/>
+      <c r="C66" s="80"/>
       <c r="D66" s="62" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
-      <c r="E66" s="95"/>
-      <c r="F66" s="80"/>
+      <c r="E66" s="107"/>
+      <c r="F66" s="83"/>
       <c r="G66" s="50"/>
-      <c r="H66" s="93"/>
-      <c r="I66" s="89"/>
+      <c r="H66" s="101"/>
+      <c r="I66" s="94"/>
       <c r="J66" s="76">
         <v>1</v>
       </c>
@@ -60421,17 +60193,17 @@
       <c r="AA66" s="18"/>
     </row>
     <row r="67" spans="1:27" s="52" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A67" s="105"/>
-      <c r="B67" s="81"/>
-      <c r="C67" s="84"/>
+      <c r="A67" s="90"/>
+      <c r="B67" s="84"/>
+      <c r="C67" s="81"/>
       <c r="D67" s="61" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
-      <c r="E67" s="96"/>
-      <c r="F67" s="81"/>
+      <c r="E67" s="108"/>
+      <c r="F67" s="84"/>
       <c r="G67" s="50"/>
-      <c r="H67" s="86"/>
-      <c r="I67" s="88"/>
+      <c r="H67" s="102"/>
+      <c r="I67" s="95"/>
       <c r="J67" s="76">
         <v>1</v>
       </c>
@@ -64810,20 +64582,102 @@
     <row r="944" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="134">
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="F58:F60"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I27:I29"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="H49:H51"/>
+    <mergeCell ref="I49:I51"/>
+    <mergeCell ref="H55:H57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="C65:C67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="H65:H67"/>
+    <mergeCell ref="I65:I67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="I58:I60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="H61:H64"/>
+    <mergeCell ref="I61:I64"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="H58:H60"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="I52:I54"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="H46:H48"/>
     <mergeCell ref="F44:F45"/>
     <mergeCell ref="E44:E45"/>
     <mergeCell ref="C46:C48"/>
@@ -64848,102 +64702,20 @@
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="H6:H9"/>
     <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="H52:H54"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="H46:H48"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="H65:H67"/>
-    <mergeCell ref="I65:I67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="I58:I60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="H61:H64"/>
-    <mergeCell ref="I61:I64"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="H58:H60"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="I10:I14"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="F58:F60"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="F65:F67"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I27:I29"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="H49:H51"/>
-    <mergeCell ref="I49:I51"/>
-    <mergeCell ref="H55:H57"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="A10:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>